<commit_message>
meta and tsla updates
</commit_message>
<xml_diff>
--- a/META/Finance Model - META (30-11-23).xlsx
+++ b/META/Finance Model - META (30-11-23).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buzz5\OneDrive\Desktop\FModels\META\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BA773BF-DB52-4B9A-9DD1-668BF28206F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C14C6D-7249-4C9D-A975-285C2CB6D754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17FDF041-F6E6-4D7C-9BBE-BB0EE7951B30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{17FDF041-F6E6-4D7C-9BBE-BB0EE7951B30}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>ALL IN $ USD</t>
   </si>
@@ -282,16 +282,16 @@
     <t>Difference</t>
   </si>
   <si>
-    <t>Market:</t>
-  </si>
-  <si>
-    <t>Net Income (Market)</t>
-  </si>
-  <si>
     <t>Cash-Debt</t>
   </si>
   <si>
     <t>11/30/2023</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Cash dividend of 0.5</t>
   </si>
 </sst>
 </file>
@@ -372,9 +372,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -713,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25291AA3-C578-4930-AA4F-F8C9E8A9B98B}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,8 +733,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>84</v>
+      <c r="A2" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -842,7 +842,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="4">
-        <v>327</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
       </c>
       <c r="D19" s="4">
         <f>D18*D17</f>
-        <v>842352</v>
+        <v>1213296</v>
       </c>
       <c r="F19" s="4"/>
     </row>
@@ -869,7 +869,7 @@
         <v>30</v>
       </c>
       <c r="D20" s="4">
-        <v>61120</v>
+        <v>65403</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="4">
-        <v>36880</v>
+        <v>35880</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
@@ -886,11 +886,21 @@
       </c>
       <c r="D22" s="4">
         <f>D19+D20-D21</f>
-        <v>866592</v>
+        <v>1242819</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A2:B8 D2:XFD8 A9:XFD1048576">
@@ -912,10 +922,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DCDFC0-4B1C-44DC-A59B-D375A632DFC2}">
-  <dimension ref="A1:GA22"/>
+  <dimension ref="A1:FV21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AS20" sqref="AS20:AS21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="AF5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,36 +948,36 @@
     <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" customWidth="1"/>
+    <col min="32" max="32" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" customWidth="1"/>
+    <col min="35" max="35" width="9" customWidth="1"/>
+    <col min="36" max="36" width="12.7109375" customWidth="1"/>
+    <col min="37" max="37" width="9.5703125" customWidth="1"/>
+    <col min="38" max="38" width="11.140625" customWidth="1"/>
     <col min="39" max="39" width="9.140625" customWidth="1"/>
-    <col min="40" max="40" width="9" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" customWidth="1"/>
-    <col min="42" max="42" width="9.5703125" customWidth="1"/>
-    <col min="43" max="43" width="11.140625" customWidth="1"/>
-    <col min="44" max="44" width="9.140625" customWidth="1"/>
-    <col min="45" max="45" width="9.42578125" customWidth="1"/>
-    <col min="46" max="46" width="10.85546875" customWidth="1"/>
-    <col min="47" max="47" width="12.5703125" customWidth="1"/>
-    <col min="48" max="48" width="14" customWidth="1"/>
-    <col min="49" max="77" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="78" max="124" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="125" max="172" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="173" max="183" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.42578125" customWidth="1"/>
+    <col min="41" max="41" width="10.85546875" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" customWidth="1"/>
+    <col min="43" max="43" width="14" customWidth="1"/>
+    <col min="44" max="44" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="72" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="119" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="120" max="167" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="168" max="178" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -972,17 +985,17 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="AK3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
     </row>
-    <row r="4" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:178" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>35</v>
       </c>
@@ -1058,126 +1071,123 @@
       <c r="AC4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AF4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL4" s="1">
-        <f t="shared" ref="AL4:AP4" si="0">AM4-1</f>
+      <c r="AG4" s="1">
+        <f t="shared" ref="AG4:AK4" si="0">AH4-1</f>
         <v>2012</v>
       </c>
-      <c r="AM4" s="1">
+      <c r="AH4" s="1">
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
-      <c r="AN4" s="1">
+      <c r="AI4" s="1">
         <f t="shared" si="0"/>
         <v>2014</v>
       </c>
-      <c r="AO4" s="1">
+      <c r="AJ4" s="1">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
-      <c r="AP4" s="1">
+      <c r="AK4" s="1">
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
+      <c r="AL4" s="1">
+        <f>AM4-1</f>
+        <v>2017</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>2018</v>
+      </c>
+      <c r="AN4" s="1">
+        <f>AM4+1</f>
+        <v>2019</v>
+      </c>
+      <c r="AO4" s="1">
+        <f t="shared" ref="AO4:BI4" si="1">AN4+1</f>
+        <v>2020</v>
+      </c>
+      <c r="AP4" s="1">
+        <f t="shared" si="1"/>
+        <v>2021</v>
+      </c>
       <c r="AQ4" s="1">
-        <f>AR4-1</f>
-        <v>2017</v>
+        <f t="shared" si="1"/>
+        <v>2022</v>
       </c>
       <c r="AR4" s="1">
-        <v>2018</v>
+        <f t="shared" si="1"/>
+        <v>2023</v>
       </c>
       <c r="AS4" s="1">
-        <f>AR4+1</f>
-        <v>2019</v>
+        <f t="shared" si="1"/>
+        <v>2024</v>
       </c>
       <c r="AT4" s="1">
-        <f t="shared" ref="AT4:BN4" si="1">AS4+1</f>
-        <v>2020</v>
+        <f t="shared" si="1"/>
+        <v>2025</v>
       </c>
       <c r="AU4" s="1">
         <f t="shared" si="1"/>
-        <v>2021</v>
+        <v>2026</v>
       </c>
       <c r="AV4" s="1">
         <f t="shared" si="1"/>
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="AW4" s="1">
         <f t="shared" si="1"/>
-        <v>2023</v>
+        <v>2028</v>
       </c>
       <c r="AX4" s="1">
         <f t="shared" si="1"/>
-        <v>2024</v>
+        <v>2029</v>
       </c>
       <c r="AY4" s="1">
         <f t="shared" si="1"/>
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="AZ4" s="1">
         <f t="shared" si="1"/>
-        <v>2026</v>
+        <v>2031</v>
       </c>
       <c r="BA4" s="1">
         <f t="shared" si="1"/>
-        <v>2027</v>
+        <v>2032</v>
       </c>
       <c r="BB4" s="1">
         <f t="shared" si="1"/>
-        <v>2028</v>
+        <v>2033</v>
       </c>
       <c r="BC4" s="1">
         <f t="shared" si="1"/>
-        <v>2029</v>
+        <v>2034</v>
       </c>
       <c r="BD4" s="1">
         <f t="shared" si="1"/>
-        <v>2030</v>
+        <v>2035</v>
       </c>
       <c r="BE4" s="1">
         <f t="shared" si="1"/>
-        <v>2031</v>
+        <v>2036</v>
       </c>
       <c r="BF4" s="1">
         <f t="shared" si="1"/>
-        <v>2032</v>
+        <v>2037</v>
       </c>
       <c r="BG4" s="1">
         <f t="shared" si="1"/>
-        <v>2033</v>
+        <v>2038</v>
       </c>
       <c r="BH4" s="1">
         <f t="shared" si="1"/>
-        <v>2034</v>
+        <v>2039</v>
       </c>
       <c r="BI4" s="1">
         <f t="shared" si="1"/>
-        <v>2035</v>
-      </c>
-      <c r="BJ4" s="1">
-        <f t="shared" si="1"/>
-        <v>2036</v>
-      </c>
-      <c r="BK4" s="1">
-        <f t="shared" si="1"/>
-        <v>2037</v>
-      </c>
-      <c r="BL4" s="1">
-        <f t="shared" si="1"/>
-        <v>2038</v>
-      </c>
-      <c r="BM4" s="1">
-        <f t="shared" si="1"/>
-        <v>2039</v>
-      </c>
-      <c r="BN4" s="1">
-        <f t="shared" si="1"/>
         <v>2040</v>
       </c>
     </row>
-    <row r="5" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>59</v>
       </c>
@@ -1255,63 +1265,64 @@
       <c r="Z5" s="4">
         <v>34146</v>
       </c>
-      <c r="AA5" s="4"/>
+      <c r="AA5" s="4">
+        <v>40111</v>
+      </c>
       <c r="AB5" s="4"/>
       <c r="AC5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="AD5" s="11">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="11">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="AH5" s="11"/>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1" t="s">
-        <v>59</v>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="4">
+        <v>5089</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>7872</v>
+      </c>
+      <c r="AI5" s="4">
+        <v>12466</v>
+      </c>
+      <c r="AJ5" s="4">
+        <v>17928</v>
+      </c>
+      <c r="AK5" s="4">
+        <v>27638</v>
       </c>
       <c r="AL5" s="4">
-        <v>5089</v>
+        <v>40653</v>
       </c>
       <c r="AM5" s="4">
-        <v>7872</v>
-      </c>
-      <c r="AN5" s="4">
-        <v>12466</v>
-      </c>
-      <c r="AO5" s="4">
-        <v>17928</v>
-      </c>
-      <c r="AP5" s="4">
-        <v>27638</v>
-      </c>
-      <c r="AQ5" s="4">
-        <v>40653</v>
-      </c>
-      <c r="AR5" s="4">
         <f>SUM(D5:G5)</f>
         <v>55838</v>
       </c>
-      <c r="AS5" s="4">
+      <c r="AN5" s="4">
         <f>SUM(H5:K5)</f>
         <v>70697</v>
       </c>
-      <c r="AT5" s="4">
+      <c r="AO5" s="4">
         <f>SUM(L5:O5)</f>
         <v>85965</v>
       </c>
-      <c r="AU5" s="4">
+      <c r="AP5" s="4">
         <f>SUM(P5:S5)</f>
         <v>117929</v>
       </c>
-      <c r="AV5" s="4">
+      <c r="AQ5" s="4">
         <f>SUM(T5:W5)</f>
         <v>116609</v>
       </c>
+      <c r="AR5" s="4">
+        <f>SUM(X5:AA5)</f>
+        <v>134901</v>
+      </c>
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
@@ -1342,13 +1353,8 @@
       <c r="BX5" s="4"/>
       <c r="BY5" s="4"/>
       <c r="BZ5" s="4"/>
-      <c r="CA5" s="4"/>
-      <c r="CB5" s="4"/>
-      <c r="CC5" s="4"/>
-      <c r="CD5" s="4"/>
-      <c r="CE5" s="4"/>
     </row>
-    <row r="6" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>60</v>
       </c>
@@ -1426,7 +1432,9 @@
       <c r="Z6" s="4">
         <v>6210</v>
       </c>
-      <c r="AA6" s="4"/>
+      <c r="AA6" s="4">
+        <v>7965</v>
+      </c>
       <c r="AB6" s="4"/>
       <c r="AC6" s="4" t="s">
         <v>75</v>
@@ -1435,53 +1443,52 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="11">
-        <v>5.5E-2</v>
-      </c>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="11"/>
-      <c r="AK6" t="s">
-        <v>60</v>
+      <c r="AG6" s="4">
+        <v>1364</v>
+      </c>
+      <c r="AH6" s="4">
+        <v>1875</v>
+      </c>
+      <c r="AI6" s="4">
+        <v>2153</v>
+      </c>
+      <c r="AJ6" s="4">
+        <v>2867</v>
+      </c>
+      <c r="AK6" s="4">
+        <v>3789</v>
       </c>
       <c r="AL6" s="4">
-        <v>1364</v>
+        <v>5454</v>
       </c>
       <c r="AM6" s="4">
-        <v>1875</v>
-      </c>
-      <c r="AN6" s="4">
-        <v>2153</v>
-      </c>
-      <c r="AO6" s="4">
-        <v>2867</v>
-      </c>
-      <c r="AP6" s="4">
-        <v>3789</v>
-      </c>
-      <c r="AQ6" s="4">
-        <v>5454</v>
-      </c>
-      <c r="AR6" s="4">
         <f>SUM(D6:G6)</f>
         <v>9355</v>
       </c>
-      <c r="AS6" s="4">
+      <c r="AN6" s="4">
         <f>SUM(H6:K6)</f>
         <v>12770</v>
       </c>
-      <c r="AT6" s="4">
+      <c r="AO6" s="4">
         <f>SUM(L6:O6)</f>
         <v>16692</v>
       </c>
-      <c r="AU6" s="4">
+      <c r="AP6" s="4">
         <f>SUM(P6:S6)</f>
         <v>22649</v>
       </c>
-      <c r="AV6" s="4">
+      <c r="AQ6" s="4">
         <f>SUM(T6:W6)</f>
         <v>25249</v>
       </c>
+      <c r="AR6" s="4">
+        <f t="shared" ref="AR6:AR14" si="2">SUM(X6:AA6)</f>
+        <v>26228</v>
+      </c>
+      <c r="AS6" s="4"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
       <c r="AW6" s="4"/>
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
@@ -1512,13 +1519,8 @@
       <c r="BX6" s="4"/>
       <c r="BY6" s="4"/>
       <c r="BZ6" s="4"/>
-      <c r="CA6" s="4"/>
-      <c r="CB6" s="4"/>
-      <c r="CC6" s="4"/>
-      <c r="CD6" s="4"/>
-      <c r="CE6" s="4"/>
     </row>
-    <row r="7" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>61</v>
       </c>
@@ -1596,64 +1598,64 @@
       <c r="Z7" s="4">
         <v>9241</v>
       </c>
-      <c r="AA7" s="4"/>
+      <c r="AA7" s="4">
+        <v>10517</v>
+      </c>
       <c r="AB7" s="4"/>
-      <c r="AC7" s="13" t="s">
+      <c r="AC7" s="12" t="s">
         <v>73</v>
       </c>
       <c r="AD7" s="4">
-        <f>NPV(AD6,AL14:GA14)</f>
-        <v>814021.23831628542</v>
+        <f>NPV(AD6,AG14:FV14)</f>
+        <v>859391.04799438466</v>
       </c>
       <c r="AE7" s="4"/>
-      <c r="AF7" s="4"/>
       <c r="AG7" s="4">
-        <f>NPV(AG6,AL15:GA15)</f>
-        <v>812998.11102043185</v>
-      </c>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="4"/>
-      <c r="AK7" t="s">
-        <v>61</v>
+        <v>1399</v>
+      </c>
+      <c r="AH7" s="4">
+        <v>1415</v>
+      </c>
+      <c r="AI7" s="4">
+        <v>2666</v>
+      </c>
+      <c r="AJ7" s="4">
+        <v>4816</v>
+      </c>
+      <c r="AK7" s="4">
+        <v>5919</v>
       </c>
       <c r="AL7" s="4">
-        <v>1399</v>
+        <v>7754</v>
       </c>
       <c r="AM7" s="4">
-        <v>1415</v>
-      </c>
-      <c r="AN7" s="4">
-        <v>2666</v>
-      </c>
-      <c r="AO7" s="4">
-        <v>4816</v>
-      </c>
-      <c r="AP7" s="4">
-        <v>5919</v>
-      </c>
-      <c r="AQ7" s="4">
-        <v>7754</v>
-      </c>
-      <c r="AR7" s="4">
         <f>SUM(D7:G7)</f>
         <v>10273</v>
       </c>
-      <c r="AS7" s="4">
+      <c r="AN7" s="4">
         <f>SUM(H7:K7)</f>
         <v>13600</v>
       </c>
-      <c r="AT7" s="4">
+      <c r="AO7" s="4">
         <f>SUM(L7:O7)</f>
         <v>18447</v>
       </c>
-      <c r="AU7" s="4">
+      <c r="AP7" s="4">
         <f>SUM(P7:S7)</f>
         <v>24655</v>
       </c>
-      <c r="AV7" s="4">
+      <c r="AQ7" s="4">
         <f>SUM(T7:W7)</f>
         <v>35338</v>
       </c>
+      <c r="AR7" s="4">
+        <f t="shared" si="2"/>
+        <v>38483</v>
+      </c>
+      <c r="AS7" s="4"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
       <c r="AW7" s="4"/>
       <c r="AX7" s="4"/>
       <c r="AY7" s="4"/>
@@ -1684,13 +1686,8 @@
       <c r="BX7" s="4"/>
       <c r="BY7" s="4"/>
       <c r="BZ7" s="4"/>
-      <c r="CA7" s="4"/>
-      <c r="CB7" s="4"/>
-      <c r="CC7" s="4"/>
-      <c r="CD7" s="4"/>
-      <c r="CE7" s="4"/>
     </row>
-    <row r="8" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>62</v>
       </c>
@@ -1768,64 +1765,64 @@
       <c r="Z8" s="4">
         <v>2877</v>
       </c>
-      <c r="AA8" s="4"/>
+      <c r="AA8" s="4">
+        <v>3226</v>
+      </c>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AD8" s="4">
         <f>Main!D20-Main!D21</f>
-        <v>24240</v>
+        <v>29523</v>
       </c>
       <c r="AE8" s="4"/>
-      <c r="AF8" s="4"/>
       <c r="AG8" s="4">
-        <f>Main!D20-Main!D21</f>
-        <v>24240</v>
-      </c>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="4"/>
-      <c r="AK8" t="s">
-        <v>62</v>
+        <v>896</v>
+      </c>
+      <c r="AH8" s="4">
+        <v>997</v>
+      </c>
+      <c r="AI8" s="4">
+        <v>1680</v>
+      </c>
+      <c r="AJ8" s="4">
+        <v>2725</v>
+      </c>
+      <c r="AK8" s="4">
+        <v>3772</v>
       </c>
       <c r="AL8" s="4">
-        <v>896</v>
+        <v>4725</v>
       </c>
       <c r="AM8" s="4">
-        <v>997</v>
-      </c>
-      <c r="AN8" s="4">
-        <v>1680</v>
-      </c>
-      <c r="AO8" s="4">
-        <v>2725</v>
-      </c>
-      <c r="AP8" s="4">
-        <v>3772</v>
-      </c>
-      <c r="AQ8" s="4">
-        <v>4725</v>
-      </c>
-      <c r="AR8" s="4">
         <f>SUM(D8:G8)</f>
         <v>7846</v>
       </c>
-      <c r="AS8" s="4">
+      <c r="AN8" s="4">
         <f>SUM(H8:K8)</f>
         <v>9876</v>
       </c>
-      <c r="AT8" s="4">
+      <c r="AO8" s="4">
         <f>SUM(L8:O8)</f>
         <v>11591</v>
       </c>
-      <c r="AU8" s="4">
+      <c r="AP8" s="4">
         <f>SUM(P8:S8)</f>
         <v>14043</v>
       </c>
-      <c r="AV8" s="4">
+      <c r="AQ8" s="4">
         <f>SUM(T8:W8)</f>
         <v>15262</v>
       </c>
+      <c r="AR8" s="4">
+        <f t="shared" si="2"/>
+        <v>12301</v>
+      </c>
+      <c r="AS8" s="4"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="4"/>
+      <c r="AV8" s="4"/>
       <c r="AW8" s="4"/>
       <c r="AX8" s="4"/>
       <c r="AY8" s="4"/>
@@ -1856,13 +1853,8 @@
       <c r="BX8" s="4"/>
       <c r="BY8" s="4"/>
       <c r="BZ8" s="4"/>
-      <c r="CA8" s="4"/>
-      <c r="CB8" s="4"/>
-      <c r="CC8" s="4"/>
-      <c r="CD8" s="4"/>
-      <c r="CE8" s="4"/>
     </row>
-    <row r="9" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>63</v>
       </c>
@@ -1940,68 +1932,65 @@
       <c r="Z9" s="4">
         <v>2070</v>
       </c>
-      <c r="AA9" s="4"/>
+      <c r="AA9" s="4">
+        <v>2289</v>
+      </c>
       <c r="AB9" s="4"/>
-      <c r="AC9" s="13" t="s">
+      <c r="AC9" s="12" t="s">
         <v>76</v>
       </c>
       <c r="AD9" s="4">
         <f>(AD7+AD8)</f>
-        <v>838261.23831628542</v>
+        <v>888914.04799438466</v>
       </c>
       <c r="AE9" s="4"/>
-      <c r="AF9" s="4"/>
       <c r="AG9" s="4">
-        <f>(AG7+AG8)</f>
-        <v>837238.11102043185</v>
-      </c>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="4"/>
-      <c r="AK9" t="s">
-        <v>63</v>
+        <v>892</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>781</v>
+      </c>
+      <c r="AI9" s="4">
+        <v>973</v>
+      </c>
+      <c r="AJ9" s="4">
+        <v>1295</v>
+      </c>
+      <c r="AK9" s="4">
+        <v>1731</v>
       </c>
       <c r="AL9" s="4">
-        <v>892</v>
+        <v>2517</v>
       </c>
       <c r="AM9" s="4">
-        <v>781</v>
-      </c>
-      <c r="AN9" s="4">
-        <v>973</v>
-      </c>
-      <c r="AO9" s="4">
-        <v>1295</v>
-      </c>
-      <c r="AP9" s="4">
-        <v>1731</v>
-      </c>
-      <c r="AQ9" s="4">
-        <v>2517</v>
-      </c>
-      <c r="AR9" s="4">
         <f>SUM(G9:J9)</f>
         <v>9611</v>
       </c>
-      <c r="AS9" s="4">
+      <c r="AN9" s="4">
         <f>SUM(D9:G9)</f>
         <v>3451</v>
       </c>
-      <c r="AT9" s="4">
+      <c r="AO9" s="4">
         <f>SUM(H9:K9)</f>
         <v>10465</v>
       </c>
-      <c r="AU9" s="4">
+      <c r="AP9" s="4">
         <f>SUM(L9:O9)</f>
         <v>6564</v>
       </c>
-      <c r="AV9" s="4">
+      <c r="AQ9" s="4">
         <f>SUM(P9:S9)</f>
         <v>9829</v>
       </c>
-      <c r="AW9" s="4">
-        <f>SUM(T9:W9)</f>
-        <v>11816</v>
-      </c>
+      <c r="AR9" s="4">
+        <f t="shared" si="2"/>
+        <v>11408</v>
+      </c>
+      <c r="AS9" s="4"/>
+      <c r="AT9" s="4"/>
+      <c r="AU9" s="4"/>
+      <c r="AV9" s="4"/>
+      <c r="AW9" s="4"/>
       <c r="AX9" s="4"/>
       <c r="AY9" s="4"/>
       <c r="AZ9" s="4"/>
@@ -2032,13 +2021,8 @@
       <c r="BY9" s="4"/>
       <c r="BZ9" s="4"/>
       <c r="CA9" s="4"/>
-      <c r="CB9" s="4"/>
-      <c r="CC9" s="4"/>
-      <c r="CD9" s="4"/>
-      <c r="CE9" s="4"/>
-      <c r="CF9" s="4"/>
     </row>
-    <row r="10" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>64</v>
       </c>
@@ -2047,153 +2031,154 @@
         <v>6517</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" ref="E10:AA10" si="2">SUM(E6:E9)</f>
+        <f t="shared" ref="E10:AA10" si="3">SUM(E6:E9)</f>
         <v>7368</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7946</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9094</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11760</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12260</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10467</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12224</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11844</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12724</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13430</v>
       </c>
       <c r="O10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15296</v>
       </c>
       <c r="P10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14793</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16710</v>
       </c>
       <c r="R10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18587</v>
       </c>
       <c r="S10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21086</v>
       </c>
       <c r="T10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19384</v>
       </c>
       <c r="U10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20464</v>
       </c>
       <c r="V10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22050</v>
       </c>
       <c r="W10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25767</v>
       </c>
       <c r="X10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21418</v>
       </c>
       <c r="Y10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22607</v>
       </c>
       <c r="Z10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20398</v>
       </c>
       <c r="AA10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>23997</v>
       </c>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
-      <c r="AF10" s="4"/>
-      <c r="AG10" s="4"/>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="4"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1" t="s">
-        <v>64</v>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="4">
+        <f t="shared" ref="AG10:AI10" si="4">SUM(AG6:AG9)</f>
+        <v>4551</v>
+      </c>
+      <c r="AH10" s="4">
+        <f t="shared" si="4"/>
+        <v>5068</v>
+      </c>
+      <c r="AI10" s="4">
+        <f t="shared" si="4"/>
+        <v>7472</v>
+      </c>
+      <c r="AJ10" s="4">
+        <f>SUM(AJ6:AJ9)</f>
+        <v>11703</v>
+      </c>
+      <c r="AK10" s="4">
+        <f t="shared" ref="AK10:AL10" si="5">SUM(AK6:AK9)</f>
+        <v>15211</v>
       </c>
       <c r="AL10" s="4">
-        <f t="shared" ref="AL10:AN10" si="3">SUM(AL6:AL9)</f>
-        <v>4551</v>
+        <f t="shared" si="5"/>
+        <v>20450</v>
       </c>
       <c r="AM10" s="4">
-        <f t="shared" si="3"/>
-        <v>5068</v>
-      </c>
-      <c r="AN10" s="4">
-        <f t="shared" si="3"/>
-        <v>7472</v>
-      </c>
-      <c r="AO10" s="4">
-        <f>SUM(AO6:AO9)</f>
-        <v>11703</v>
-      </c>
-      <c r="AP10" s="4">
-        <f t="shared" ref="AP10:AQ10" si="4">SUM(AP6:AP9)</f>
-        <v>15211</v>
-      </c>
-      <c r="AQ10" s="4">
-        <f t="shared" si="4"/>
-        <v>20450</v>
-      </c>
-      <c r="AR10" s="4">
         <f>SUM(D10:G10)</f>
         <v>30925</v>
       </c>
-      <c r="AS10" s="4">
+      <c r="AN10" s="4">
         <f>SUM(H10:K10)</f>
         <v>46711</v>
       </c>
-      <c r="AT10" s="4">
+      <c r="AO10" s="4">
         <f>SUM(L10:O10)</f>
         <v>53294</v>
       </c>
-      <c r="AU10" s="4">
+      <c r="AP10" s="4">
         <f>SUM(P10:S10)</f>
         <v>71176</v>
       </c>
-      <c r="AV10" s="4">
+      <c r="AQ10" s="4">
         <f>SUM(T10:W10)</f>
         <v>87665</v>
       </c>
+      <c r="AR10" s="4">
+        <f t="shared" si="2"/>
+        <v>88420</v>
+      </c>
+      <c r="AS10" s="4"/>
+      <c r="AT10" s="4"/>
+      <c r="AU10" s="4"/>
+      <c r="AV10" s="4"/>
       <c r="AW10" s="4"/>
       <c r="AX10" s="4"/>
       <c r="AY10" s="4"/>
@@ -2224,13 +2209,8 @@
       <c r="BX10" s="4"/>
       <c r="BY10" s="4"/>
       <c r="BZ10" s="4"/>
-      <c r="CA10" s="4"/>
-      <c r="CB10" s="4"/>
-      <c r="CC10" s="4"/>
-      <c r="CD10" s="4"/>
-      <c r="CE10" s="4"/>
     </row>
-    <row r="11" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>65</v>
       </c>
@@ -2239,96 +2219,96 @@
         <v>5449</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" ref="E11:AA11" si="5">E5-E10</f>
+        <f t="shared" ref="E11:AA11" si="6">E5-E10</f>
         <v>5863</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5781</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7820</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3317</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4626</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7185</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8858</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5893</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5963</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8040</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12775</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11378</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12367</v>
       </c>
       <c r="R11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10423</v>
       </c>
       <c r="S11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12585</v>
       </c>
       <c r="T11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8524</v>
       </c>
       <c r="U11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8358</v>
       </c>
       <c r="V11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5664</v>
       </c>
       <c r="W11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6398</v>
       </c>
       <c r="X11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7227</v>
       </c>
       <c r="Y11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9392</v>
       </c>
       <c r="Z11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13748</v>
       </c>
       <c r="AA11" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>16114</v>
       </c>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4" t="s">
@@ -2336,64 +2316,62 @@
       </c>
       <c r="AD11" s="4">
         <f>Main!D17</f>
-        <v>327</v>
+        <v>471</v>
       </c>
       <c r="AE11" s="4"/>
-      <c r="AF11" s="4"/>
+      <c r="AF11" s="1"/>
       <c r="AG11" s="4">
-        <f>Main!D17</f>
-        <v>327</v>
-      </c>
-      <c r="AH11" s="4"/>
-      <c r="AI11" s="4"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1" t="s">
-        <v>65</v>
+        <f t="shared" ref="AG11:AI11" si="7">AG5-AG10</f>
+        <v>538</v>
+      </c>
+      <c r="AH11" s="4">
+        <f t="shared" si="7"/>
+        <v>2804</v>
+      </c>
+      <c r="AI11" s="4">
+        <f t="shared" si="7"/>
+        <v>4994</v>
+      </c>
+      <c r="AJ11" s="4">
+        <f>AJ5-AJ10</f>
+        <v>6225</v>
+      </c>
+      <c r="AK11" s="4">
+        <f t="shared" ref="AK11:AL11" si="8">AK5-AK10</f>
+        <v>12427</v>
       </c>
       <c r="AL11" s="4">
-        <f t="shared" ref="AL11:AN11" si="6">AL5-AL10</f>
-        <v>538</v>
+        <f t="shared" si="8"/>
+        <v>20203</v>
       </c>
       <c r="AM11" s="4">
-        <f t="shared" si="6"/>
-        <v>2804</v>
-      </c>
-      <c r="AN11" s="4">
-        <f t="shared" si="6"/>
-        <v>4994</v>
-      </c>
-      <c r="AO11" s="4">
-        <f>AO5-AO10</f>
-        <v>6225</v>
-      </c>
-      <c r="AP11" s="4">
-        <f t="shared" ref="AP11:AQ11" si="7">AP5-AP10</f>
-        <v>12427</v>
-      </c>
-      <c r="AQ11" s="4">
-        <f t="shared" si="7"/>
-        <v>20203</v>
-      </c>
-      <c r="AR11" s="4">
         <f>SUM(D11:G11)</f>
         <v>24913</v>
       </c>
-      <c r="AS11" s="4">
+      <c r="AN11" s="4">
         <f>SUM(H11:K11)</f>
         <v>23986</v>
       </c>
-      <c r="AT11" s="4">
+      <c r="AO11" s="4">
         <f>SUM(L11:O11)</f>
         <v>32671</v>
       </c>
-      <c r="AU11" s="4">
+      <c r="AP11" s="4">
         <f>SUM(P11:S11)</f>
         <v>46753</v>
       </c>
-      <c r="AV11" s="4">
+      <c r="AQ11" s="4">
         <f>SUM(T11:W11)</f>
         <v>28944</v>
       </c>
+      <c r="AR11" s="4">
+        <f t="shared" si="2"/>
+        <v>46481</v>
+      </c>
+      <c r="AS11" s="4"/>
+      <c r="AT11" s="4"/>
+      <c r="AU11" s="4"/>
+      <c r="AV11" s="4"/>
       <c r="AW11" s="4"/>
       <c r="AX11" s="4"/>
       <c r="AY11" s="4"/>
@@ -2424,13 +2402,8 @@
       <c r="BX11" s="4"/>
       <c r="BY11" s="4"/>
       <c r="BZ11" s="4"/>
-      <c r="CA11" s="4"/>
-      <c r="CB11" s="4"/>
-      <c r="CC11" s="4"/>
-      <c r="CD11" s="4"/>
-      <c r="CE11" s="4"/>
     </row>
-    <row r="12" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>66</v>
       </c>
@@ -2508,64 +2481,64 @@
       <c r="Z12" s="4">
         <v>272</v>
       </c>
-      <c r="AA12" s="4"/>
+      <c r="AA12" s="4">
+        <v>424</v>
+      </c>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4" t="s">
         <v>79</v>
       </c>
       <c r="AD12" s="4">
         <f>AD9/Main!D18</f>
-        <v>325.41197139607351</v>
+        <v>345.07532919036669</v>
       </c>
       <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
       <c r="AG12" s="4">
-        <f>AG9/Main!D18</f>
-        <v>325.01479465078876</v>
-      </c>
-      <c r="AH12" s="4"/>
-      <c r="AI12" s="4"/>
-      <c r="AK12" t="s">
-        <v>66</v>
+        <v>7</v>
+      </c>
+      <c r="AH12" s="4">
+        <v>-50</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>-84</v>
+      </c>
+      <c r="AJ12" s="4">
+        <v>-31</v>
+      </c>
+      <c r="AK12" s="4">
+        <v>91</v>
       </c>
       <c r="AL12" s="4">
-        <v>7</v>
+        <v>391</v>
       </c>
       <c r="AM12" s="4">
-        <v>-50</v>
-      </c>
-      <c r="AN12" s="4">
-        <v>-84</v>
-      </c>
-      <c r="AO12" s="4">
-        <v>-31</v>
-      </c>
-      <c r="AP12" s="4">
-        <v>91</v>
-      </c>
-      <c r="AQ12" s="4">
-        <v>391</v>
-      </c>
-      <c r="AR12" s="4">
         <f>SUM(D12:G12)</f>
         <v>448</v>
       </c>
-      <c r="AS12" s="4">
+      <c r="AN12" s="4">
         <f>SUM(H12:K12)</f>
         <v>826</v>
       </c>
-      <c r="AT12" s="4">
+      <c r="AO12" s="4">
         <f>SUM(L12:O12)</f>
         <v>445</v>
       </c>
-      <c r="AU12" s="4">
+      <c r="AP12" s="4">
         <f>SUM(P12:S12)</f>
         <v>531</v>
       </c>
-      <c r="AV12" s="4">
+      <c r="AQ12" s="4">
         <f>SUM(T12:W12)</f>
         <v>123</v>
       </c>
+      <c r="AR12" s="4">
+        <f t="shared" si="2"/>
+        <v>677</v>
+      </c>
+      <c r="AS12" s="4"/>
+      <c r="AT12" s="4"/>
+      <c r="AU12" s="4"/>
+      <c r="AV12" s="4"/>
       <c r="AW12" s="4"/>
       <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
@@ -2596,13 +2569,8 @@
       <c r="BX12" s="4"/>
       <c r="BY12" s="4"/>
       <c r="BZ12" s="4"/>
-      <c r="CA12" s="4"/>
-      <c r="CB12" s="4"/>
-      <c r="CC12" s="4"/>
-      <c r="CD12" s="4"/>
-      <c r="CE12" s="4"/>
     </row>
-    <row r="13" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>67</v>
       </c>
@@ -2680,64 +2648,64 @@
       <c r="Z13" s="4">
         <v>2437</v>
       </c>
-      <c r="AA13" s="4"/>
+      <c r="AA13" s="4">
+        <v>2791</v>
+      </c>
       <c r="AB13" s="4"/>
       <c r="AC13" s="4" t="s">
         <v>80</v>
       </c>
       <c r="AD13" s="10">
         <f>AD12/AD11-1</f>
-        <v>-4.8563565869311764E-3</v>
+        <v>-0.26735598898011315</v>
       </c>
       <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
-      <c r="AG13" s="11">
-        <f>AG12/AG11-1</f>
-        <v>-6.070964370676557E-3</v>
-      </c>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AK13" t="s">
-        <v>67</v>
+      <c r="AG13" s="4">
+        <v>441</v>
+      </c>
+      <c r="AH13" s="4">
+        <v>1254</v>
+      </c>
+      <c r="AI13" s="4">
+        <v>1970</v>
+      </c>
+      <c r="AJ13" s="4">
+        <v>2506</v>
+      </c>
+      <c r="AK13" s="4">
+        <v>2301</v>
       </c>
       <c r="AL13" s="4">
-        <v>441</v>
+        <v>4660</v>
       </c>
       <c r="AM13" s="4">
-        <v>1254</v>
-      </c>
-      <c r="AN13" s="4">
-        <v>1970</v>
-      </c>
-      <c r="AO13" s="4">
-        <v>2506</v>
-      </c>
-      <c r="AP13" s="4">
-        <v>2301</v>
-      </c>
-      <c r="AQ13" s="4">
-        <v>4660</v>
-      </c>
-      <c r="AR13" s="4">
         <f>SUM(D13:G13)</f>
         <v>3249</v>
       </c>
-      <c r="AS13" s="4">
+      <c r="AN13" s="4">
         <f>SUM(H13:K13)</f>
         <v>6327</v>
       </c>
-      <c r="AT13" s="4">
+      <c r="AO13" s="4">
         <f>SUM(L13:O13)</f>
         <v>4034</v>
       </c>
-      <c r="AU13" s="4">
+      <c r="AP13" s="4">
         <f>SUM(P13:S13)</f>
         <v>7914</v>
       </c>
-      <c r="AV13" s="4">
+      <c r="AQ13" s="4">
         <f>SUM(T13:W13)</f>
         <v>5619</v>
       </c>
+      <c r="AR13" s="4">
+        <f t="shared" si="2"/>
+        <v>8331</v>
+      </c>
+      <c r="AS13" s="4"/>
+      <c r="AT13" s="4"/>
+      <c r="AU13" s="4"/>
+      <c r="AV13" s="4"/>
       <c r="AW13" s="4"/>
       <c r="AX13" s="4"/>
       <c r="AY13" s="4"/>
@@ -2768,13 +2736,8 @@
       <c r="BX13" s="4"/>
       <c r="BY13" s="4"/>
       <c r="BZ13" s="4"/>
-      <c r="CA13" s="4"/>
-      <c r="CB13" s="4"/>
-      <c r="CC13" s="4"/>
-      <c r="CD13" s="4"/>
-      <c r="CE13" s="4"/>
     </row>
-    <row r="14" spans="1:183" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:178" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>68</v>
       </c>
@@ -2783,1759 +2746,1314 @@
         <v>4988</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" ref="E14:AA14" si="8">E11+E12-E13</f>
+        <f t="shared" ref="E14:AA14" si="9">E11+E12-E13</f>
         <v>5106</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5137</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6881</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2429</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2616</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6091</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7349</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4902</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5178</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7846</v>
       </c>
       <c r="O14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11156</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9497</v>
       </c>
       <c r="Q14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10394</v>
       </c>
       <c r="R14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9194</v>
       </c>
       <c r="S14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10285</v>
       </c>
       <c r="T14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7465</v>
       </c>
       <c r="U14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6687</v>
       </c>
       <c r="V14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4395</v>
       </c>
       <c r="W14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4901</v>
       </c>
       <c r="X14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5709</v>
       </c>
       <c r="Y14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7788</v>
       </c>
       <c r="Z14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11583</v>
       </c>
       <c r="AA14" s="4">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>13747</v>
       </c>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
-      <c r="AF14" s="4"/>
-      <c r="AG14" s="4"/>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="4"/>
-      <c r="AJ14" s="1"/>
-      <c r="AK14" s="1" t="s">
-        <v>68</v>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="4">
+        <f t="shared" ref="AG14:AI14" si="10">AG10+AG12-AG13</f>
+        <v>4117</v>
+      </c>
+      <c r="AH14" s="4">
+        <f t="shared" si="10"/>
+        <v>3764</v>
+      </c>
+      <c r="AI14" s="4">
+        <f t="shared" si="10"/>
+        <v>5418</v>
+      </c>
+      <c r="AJ14" s="4">
+        <f>AJ10+AJ12-AJ13</f>
+        <v>9166</v>
+      </c>
+      <c r="AK14" s="4">
+        <f t="shared" ref="AK14:AL14" si="11">AK10+AK12-AK13</f>
+        <v>13001</v>
       </c>
       <c r="AL14" s="4">
-        <f t="shared" ref="AL14:AN14" si="9">AL10+AL12-AL13</f>
-        <v>4117</v>
+        <f t="shared" si="11"/>
+        <v>16181</v>
       </c>
       <c r="AM14" s="4">
-        <f t="shared" si="9"/>
-        <v>3764</v>
-      </c>
-      <c r="AN14" s="4">
-        <f t="shared" si="9"/>
-        <v>5418</v>
-      </c>
-      <c r="AO14" s="4">
-        <f>AO10+AO12-AO13</f>
-        <v>9166</v>
-      </c>
-      <c r="AP14" s="4">
-        <f t="shared" ref="AP14:AQ14" si="10">AP10+AP12-AP13</f>
-        <v>13001</v>
-      </c>
-      <c r="AQ14" s="4">
-        <f t="shared" si="10"/>
-        <v>16181</v>
-      </c>
-      <c r="AR14" s="4">
         <f>SUM(D14:G14)</f>
         <v>22112</v>
       </c>
-      <c r="AS14" s="4">
+      <c r="AN14" s="4">
         <f>SUM(H14:K14)</f>
         <v>18485</v>
       </c>
-      <c r="AT14" s="4">
+      <c r="AO14" s="4">
         <f>SUM(L14:O14)</f>
         <v>29082</v>
       </c>
-      <c r="AU14" s="4">
+      <c r="AP14" s="4">
         <f>SUM(P14:S14)</f>
         <v>39370</v>
       </c>
-      <c r="AV14" s="4">
+      <c r="AQ14" s="4">
         <f>SUM(T14:W14)</f>
         <v>23448</v>
       </c>
+      <c r="AR14" s="4">
+        <f t="shared" si="2"/>
+        <v>38827</v>
+      </c>
+      <c r="AS14" s="4">
+        <f>AR14*($AD5+1)</f>
+        <v>40380.080000000002</v>
+      </c>
+      <c r="AT14" s="4">
+        <f t="shared" ref="AT14:DE14" si="12">AS14*($AD5+1)</f>
+        <v>41995.283200000005</v>
+      </c>
+      <c r="AU14" s="4">
+        <f t="shared" si="12"/>
+        <v>43675.094528000009</v>
+      </c>
+      <c r="AV14" s="4">
+        <f t="shared" si="12"/>
+        <v>45422.098309120011</v>
+      </c>
       <c r="AW14" s="4">
-        <f>AV14*($AD5+1)</f>
-        <v>24620.400000000001</v>
+        <f t="shared" si="12"/>
+        <v>47238.982241484809</v>
       </c>
       <c r="AX14" s="4">
-        <f>AW14*($AD5+1)</f>
-        <v>25851.420000000002</v>
+        <f t="shared" si="12"/>
+        <v>49128.541531144205</v>
       </c>
       <c r="AY14" s="4">
-        <f t="shared" ref="AY14:DJ14" si="11">AX14*($AD5+1)</f>
-        <v>27143.991000000002</v>
+        <f t="shared" si="12"/>
+        <v>51093.683192389974</v>
       </c>
       <c r="AZ14" s="4">
-        <f t="shared" si="11"/>
-        <v>28501.190550000003</v>
+        <f t="shared" si="12"/>
+        <v>53137.430520085574</v>
       </c>
       <c r="BA14" s="4">
-        <f t="shared" si="11"/>
-        <v>29926.250077500004</v>
+        <f t="shared" si="12"/>
+        <v>55262.927740888998</v>
       </c>
       <c r="BB14" s="4">
-        <f t="shared" si="11"/>
-        <v>31422.562581375005</v>
+        <f t="shared" si="12"/>
+        <v>57473.44485052456</v>
       </c>
       <c r="BC14" s="4">
-        <f t="shared" si="11"/>
-        <v>32993.690710443756</v>
+        <f t="shared" si="12"/>
+        <v>59772.382644545542</v>
       </c>
       <c r="BD14" s="4">
-        <f t="shared" si="11"/>
-        <v>34643.375245965944</v>
+        <f t="shared" si="12"/>
+        <v>62163.277950327363</v>
       </c>
       <c r="BE14" s="4">
-        <f t="shared" si="11"/>
-        <v>36375.544008264245</v>
+        <f t="shared" si="12"/>
+        <v>64649.809068340459</v>
       </c>
       <c r="BF14" s="4">
-        <f t="shared" si="11"/>
-        <v>38194.321208677458</v>
+        <f t="shared" si="12"/>
+        <v>67235.801431074084</v>
       </c>
       <c r="BG14" s="4">
-        <f t="shared" si="11"/>
-        <v>40104.03726911133</v>
+        <f t="shared" si="12"/>
+        <v>69925.233488317055</v>
       </c>
       <c r="BH14" s="4">
-        <f t="shared" si="11"/>
-        <v>42109.239132566901</v>
+        <f t="shared" si="12"/>
+        <v>72722.242827849739</v>
       </c>
       <c r="BI14" s="4">
-        <f t="shared" si="11"/>
-        <v>44214.701089195245</v>
+        <f t="shared" si="12"/>
+        <v>75631.132540963736</v>
       </c>
       <c r="BJ14" s="4">
-        <f t="shared" si="11"/>
-        <v>46425.43614365501</v>
+        <f t="shared" si="12"/>
+        <v>78656.377842602291</v>
       </c>
       <c r="BK14" s="4">
-        <f t="shared" si="11"/>
-        <v>48746.707950837765</v>
+        <f t="shared" si="12"/>
+        <v>81802.632956306392</v>
       </c>
       <c r="BL14" s="4">
-        <f t="shared" si="11"/>
-        <v>51184.043348379651</v>
+        <f t="shared" si="12"/>
+        <v>85074.738274558651</v>
       </c>
       <c r="BM14" s="4">
-        <f t="shared" si="11"/>
-        <v>53743.245515798633</v>
+        <f t="shared" si="12"/>
+        <v>88477.727805540999</v>
       </c>
       <c r="BN14" s="4">
-        <f t="shared" si="11"/>
-        <v>56430.407791588565</v>
+        <f t="shared" si="12"/>
+        <v>92016.836917762645</v>
       </c>
       <c r="BO14" s="4">
-        <f t="shared" si="11"/>
-        <v>59251.928181167998</v>
+        <f t="shared" si="12"/>
+        <v>95697.510394473153</v>
       </c>
       <c r="BP14" s="4">
-        <f t="shared" si="11"/>
-        <v>62214.5245902264</v>
+        <f t="shared" si="12"/>
+        <v>99525.410810252084</v>
       </c>
       <c r="BQ14" s="4">
-        <f t="shared" si="11"/>
-        <v>65325.250819737725</v>
+        <f t="shared" si="12"/>
+        <v>103506.42724266218</v>
       </c>
       <c r="BR14" s="4">
-        <f t="shared" si="11"/>
-        <v>68591.51336072461</v>
+        <f t="shared" si="12"/>
+        <v>107646.68433236866</v>
       </c>
       <c r="BS14" s="4">
-        <f t="shared" si="11"/>
-        <v>72021.089028760849</v>
+        <f t="shared" si="12"/>
+        <v>111952.55170566341</v>
       </c>
       <c r="BT14" s="4">
-        <f t="shared" si="11"/>
-        <v>75622.143480198894</v>
+        <f t="shared" si="12"/>
+        <v>116430.65377388995</v>
       </c>
       <c r="BU14" s="4">
-        <f t="shared" si="11"/>
-        <v>79403.250654208838</v>
+        <f t="shared" si="12"/>
+        <v>121087.87992484555</v>
       </c>
       <c r="BV14" s="4">
-        <f t="shared" si="11"/>
-        <v>83373.413186919279</v>
+        <f t="shared" si="12"/>
+        <v>125931.39512183938</v>
       </c>
       <c r="BW14" s="4">
-        <f t="shared" si="11"/>
-        <v>87542.083846265246</v>
+        <f t="shared" si="12"/>
+        <v>130968.65092671296</v>
       </c>
       <c r="BX14" s="4">
-        <f t="shared" si="11"/>
-        <v>91919.188038578519</v>
+        <f t="shared" si="12"/>
+        <v>136207.39696378147</v>
       </c>
       <c r="BY14" s="4">
-        <f t="shared" si="11"/>
-        <v>96515.147440507455</v>
+        <f t="shared" si="12"/>
+        <v>141655.69284233273</v>
       </c>
       <c r="BZ14" s="4">
-        <f t="shared" si="11"/>
-        <v>101340.90481253283</v>
+        <f t="shared" si="12"/>
+        <v>147321.92055602605</v>
       </c>
       <c r="CA14" s="4">
-        <f t="shared" si="11"/>
-        <v>106407.95005315947</v>
+        <f t="shared" si="12"/>
+        <v>153214.7973782671</v>
       </c>
       <c r="CB14" s="4">
-        <f t="shared" si="11"/>
-        <v>111728.34755581744</v>
+        <f t="shared" si="12"/>
+        <v>159343.3892733978</v>
       </c>
       <c r="CC14" s="4">
-        <f t="shared" si="11"/>
-        <v>117314.76493360831</v>
+        <f t="shared" si="12"/>
+        <v>165717.12484433371</v>
       </c>
       <c r="CD14" s="4">
-        <f t="shared" si="11"/>
-        <v>123180.50318028874</v>
+        <f t="shared" si="12"/>
+        <v>172345.80983810706</v>
       </c>
       <c r="CE14" s="4">
-        <f t="shared" si="11"/>
-        <v>129339.52833930319</v>
+        <f t="shared" si="12"/>
+        <v>179239.64223163135</v>
       </c>
       <c r="CF14" s="4">
-        <f t="shared" si="11"/>
-        <v>135806.50475626835</v>
+        <f t="shared" si="12"/>
+        <v>186409.22792089661</v>
       </c>
       <c r="CG14" s="4">
-        <f t="shared" si="11"/>
-        <v>142596.82999408178</v>
+        <f t="shared" si="12"/>
+        <v>193865.59703773248</v>
       </c>
       <c r="CH14" s="4">
-        <f t="shared" si="11"/>
-        <v>149726.67149378586</v>
+        <f t="shared" si="12"/>
+        <v>201620.22091924178</v>
       </c>
       <c r="CI14" s="4">
-        <f t="shared" si="11"/>
-        <v>157213.00506847518</v>
+        <f t="shared" si="12"/>
+        <v>209685.02975601147</v>
       </c>
       <c r="CJ14" s="4">
-        <f t="shared" si="11"/>
-        <v>165073.65532189893</v>
+        <f t="shared" si="12"/>
+        <v>218072.43094625193</v>
       </c>
       <c r="CK14" s="4">
-        <f t="shared" si="11"/>
-        <v>173327.33808799388</v>
+        <f t="shared" si="12"/>
+        <v>226795.32818410202</v>
       </c>
       <c r="CL14" s="4">
-        <f t="shared" si="11"/>
-        <v>181993.70499239358</v>
+        <f t="shared" si="12"/>
+        <v>235867.14131146611</v>
       </c>
       <c r="CM14" s="4">
-        <f t="shared" si="11"/>
-        <v>191093.39024201327</v>
+        <f t="shared" si="12"/>
+        <v>245301.82696392477</v>
       </c>
       <c r="CN14" s="4">
-        <f t="shared" si="11"/>
-        <v>200648.05975411393</v>
+        <f t="shared" si="12"/>
+        <v>255113.90004248178</v>
       </c>
       <c r="CO14" s="4">
-        <f t="shared" si="11"/>
-        <v>210680.46274181965</v>
+        <f t="shared" si="12"/>
+        <v>265318.45604418108</v>
       </c>
       <c r="CP14" s="4">
-        <f t="shared" si="11"/>
-        <v>221214.48587891064</v>
+        <f t="shared" si="12"/>
+        <v>275931.19428594835</v>
       </c>
       <c r="CQ14" s="4">
-        <f t="shared" si="11"/>
-        <v>232275.21017285617</v>
+        <f t="shared" si="12"/>
+        <v>286968.44205738627</v>
       </c>
       <c r="CR14" s="4">
-        <f t="shared" si="11"/>
-        <v>243888.97068149899</v>
+        <f t="shared" si="12"/>
+        <v>298447.17973968171</v>
       </c>
       <c r="CS14" s="4">
-        <f t="shared" si="11"/>
-        <v>256083.41921557396</v>
+        <f t="shared" si="12"/>
+        <v>310385.066929269</v>
       </c>
       <c r="CT14" s="4">
-        <f t="shared" si="11"/>
-        <v>268887.59017635265</v>
+        <f t="shared" si="12"/>
+        <v>322800.46960643976</v>
       </c>
       <c r="CU14" s="4">
-        <f t="shared" si="11"/>
-        <v>282331.96968517028</v>
+        <f t="shared" si="12"/>
+        <v>335712.48839069734</v>
       </c>
       <c r="CV14" s="4">
-        <f t="shared" si="11"/>
-        <v>296448.56816942879</v>
+        <f t="shared" si="12"/>
+        <v>349140.98792632524</v>
       </c>
       <c r="CW14" s="4">
-        <f t="shared" si="11"/>
-        <v>311270.99657790025</v>
+        <f t="shared" si="12"/>
+        <v>363106.62744337827</v>
       </c>
       <c r="CX14" s="4">
-        <f t="shared" si="11"/>
-        <v>326834.54640679527</v>
+        <f t="shared" si="12"/>
+        <v>377630.89254111343</v>
       </c>
       <c r="CY14" s="4">
-        <f t="shared" si="11"/>
-        <v>343176.27372713503</v>
+        <f t="shared" si="12"/>
+        <v>392736.12824275799</v>
       </c>
       <c r="CZ14" s="4">
-        <f t="shared" si="11"/>
-        <v>360335.0874134918</v>
+        <f t="shared" si="12"/>
+        <v>408445.57337246829</v>
       </c>
       <c r="DA14" s="4">
-        <f t="shared" si="11"/>
-        <v>378351.8417841664</v>
+        <f t="shared" si="12"/>
+        <v>424783.39630736702</v>
       </c>
       <c r="DB14" s="4">
-        <f t="shared" si="11"/>
-        <v>397269.43387337471</v>
+        <f t="shared" si="12"/>
+        <v>441774.73215966171</v>
       </c>
       <c r="DC14" s="4">
-        <f t="shared" si="11"/>
-        <v>417132.90556704346</v>
+        <f t="shared" si="12"/>
+        <v>459445.72144604818</v>
       </c>
       <c r="DD14" s="4">
-        <f t="shared" si="11"/>
-        <v>437989.55084539566</v>
+        <f t="shared" si="12"/>
+        <v>477823.55030389014</v>
       </c>
       <c r="DE14" s="4">
-        <f t="shared" si="11"/>
-        <v>459889.02838766546</v>
+        <f t="shared" si="12"/>
+        <v>496936.49231604574</v>
       </c>
       <c r="DF14" s="4">
-        <f t="shared" si="11"/>
-        <v>482883.47980704874</v>
+        <f t="shared" ref="DF14:FQ14" si="13">DE14*($AD5+1)</f>
+        <v>516813.9520086876</v>
       </c>
       <c r="DG14" s="4">
-        <f t="shared" si="11"/>
-        <v>507027.65379740123</v>
+        <f t="shared" si="13"/>
+        <v>537486.51008903515</v>
       </c>
       <c r="DH14" s="4">
-        <f t="shared" si="11"/>
-        <v>532379.03648727131</v>
+        <f t="shared" si="13"/>
+        <v>558985.97049259662</v>
       </c>
       <c r="DI14" s="4">
-        <f t="shared" si="11"/>
-        <v>558997.98831163486</v>
+        <f t="shared" si="13"/>
+        <v>581345.4093123005</v>
       </c>
       <c r="DJ14" s="4">
-        <f t="shared" si="11"/>
-        <v>586947.88772721658</v>
+        <f t="shared" si="13"/>
+        <v>604599.2256847925</v>
       </c>
       <c r="DK14" s="4">
-        <f t="shared" ref="DK14:FV14" si="12">DJ14*($AD5+1)</f>
-        <v>616295.28211357747</v>
+        <f t="shared" si="13"/>
+        <v>628783.19471218425</v>
       </c>
       <c r="DL14" s="4">
-        <f t="shared" si="12"/>
-        <v>647110.04621925636</v>
+        <f t="shared" si="13"/>
+        <v>653934.52250067168</v>
       </c>
       <c r="DM14" s="4">
-        <f t="shared" si="12"/>
-        <v>679465.54853021924</v>
+        <f t="shared" si="13"/>
+        <v>680091.90340069856</v>
       </c>
       <c r="DN14" s="4">
-        <f t="shared" si="12"/>
-        <v>713438.82595673029</v>
+        <f t="shared" si="13"/>
+        <v>707295.57953672658</v>
       </c>
       <c r="DO14" s="4">
-        <f t="shared" si="12"/>
-        <v>749110.76725456689</v>
+        <f t="shared" si="13"/>
+        <v>735587.40271819569</v>
       </c>
       <c r="DP14" s="4">
-        <f t="shared" si="12"/>
-        <v>786566.30561729532</v>
+        <f t="shared" si="13"/>
+        <v>765010.89882692357</v>
       </c>
       <c r="DQ14" s="4">
-        <f t="shared" si="12"/>
-        <v>825894.62089816015</v>
+        <f t="shared" si="13"/>
+        <v>795611.3347800005</v>
       </c>
       <c r="DR14" s="4">
-        <f t="shared" si="12"/>
-        <v>867189.35194306821</v>
+        <f t="shared" si="13"/>
+        <v>827435.78817120055</v>
       </c>
       <c r="DS14" s="4">
-        <f t="shared" si="12"/>
-        <v>910548.81954022171</v>
+        <f t="shared" si="13"/>
+        <v>860533.21969804855</v>
       </c>
       <c r="DT14" s="4">
-        <f t="shared" si="12"/>
-        <v>956076.26051723282</v>
+        <f t="shared" si="13"/>
+        <v>894954.54848597047</v>
       </c>
       <c r="DU14" s="4">
-        <f t="shared" si="12"/>
-        <v>1003880.0735430944</v>
+        <f t="shared" si="13"/>
+        <v>930752.73042540927</v>
       </c>
       <c r="DV14" s="4">
-        <f t="shared" si="12"/>
-        <v>1054074.0772202492</v>
+        <f t="shared" si="13"/>
+        <v>967982.83964242565</v>
       </c>
       <c r="DW14" s="4">
-        <f t="shared" si="12"/>
-        <v>1106777.7810812618</v>
+        <f t="shared" si="13"/>
+        <v>1006702.1532281227</v>
       </c>
       <c r="DX14" s="4">
-        <f t="shared" si="12"/>
-        <v>1162116.6701353251</v>
+        <f t="shared" si="13"/>
+        <v>1046970.2393572477</v>
       </c>
       <c r="DY14" s="4">
-        <f t="shared" si="12"/>
-        <v>1220222.5036420913</v>
+        <f t="shared" si="13"/>
+        <v>1088849.0489315377</v>
       </c>
       <c r="DZ14" s="4">
-        <f t="shared" si="12"/>
-        <v>1281233.6288241958</v>
+        <f t="shared" si="13"/>
+        <v>1132403.0108887991</v>
       </c>
       <c r="EA14" s="4">
-        <f t="shared" si="12"/>
-        <v>1345295.3102654056</v>
+        <f t="shared" si="13"/>
+        <v>1177699.1313243511</v>
       </c>
       <c r="EB14" s="4">
-        <f t="shared" si="12"/>
-        <v>1412560.075778676</v>
+        <f t="shared" si="13"/>
+        <v>1224807.0965773251</v>
       </c>
       <c r="EC14" s="4">
-        <f t="shared" si="12"/>
-        <v>1483188.0795676098</v>
+        <f t="shared" si="13"/>
+        <v>1273799.3804404181</v>
       </c>
       <c r="ED14" s="4">
-        <f t="shared" si="12"/>
-        <v>1557347.4835459904</v>
+        <f t="shared" si="13"/>
+        <v>1324751.355658035</v>
       </c>
       <c r="EE14" s="4">
-        <f t="shared" si="12"/>
-        <v>1635214.8577232901</v>
+        <f t="shared" si="13"/>
+        <v>1377741.4098843564</v>
       </c>
       <c r="EF14" s="4">
-        <f t="shared" si="12"/>
-        <v>1716975.6006094548</v>
+        <f t="shared" si="13"/>
+        <v>1432851.0662797308</v>
       </c>
       <c r="EG14" s="4">
-        <f t="shared" si="12"/>
-        <v>1802824.3806399277</v>
+        <f t="shared" si="13"/>
+        <v>1490165.10893092</v>
       </c>
       <c r="EH14" s="4">
-        <f t="shared" si="12"/>
-        <v>1892965.5996719243</v>
+        <f t="shared" si="13"/>
+        <v>1549771.7132881568</v>
       </c>
       <c r="EI14" s="4">
-        <f t="shared" si="12"/>
-        <v>1987613.8796555207</v>
+        <f t="shared" si="13"/>
+        <v>1611762.5818196831</v>
       </c>
       <c r="EJ14" s="4">
-        <f t="shared" si="12"/>
-        <v>2086994.5736382967</v>
+        <f t="shared" si="13"/>
+        <v>1676233.0850924705</v>
       </c>
       <c r="EK14" s="4">
-        <f t="shared" si="12"/>
-        <v>2191344.3023202117</v>
+        <f t="shared" si="13"/>
+        <v>1743282.4084961694</v>
       </c>
       <c r="EL14" s="4">
-        <f t="shared" si="12"/>
-        <v>2300911.5174362222</v>
+        <f t="shared" si="13"/>
+        <v>1813013.7048360163</v>
       </c>
       <c r="EM14" s="4">
-        <f t="shared" si="12"/>
-        <v>2415957.0933080334</v>
+        <f t="shared" si="13"/>
+        <v>1885534.2530294571</v>
       </c>
       <c r="EN14" s="4">
-        <f t="shared" si="12"/>
-        <v>2536754.9479734353</v>
+        <f t="shared" si="13"/>
+        <v>1960955.6231506355</v>
       </c>
       <c r="EO14" s="4">
-        <f t="shared" si="12"/>
-        <v>2663592.695372107</v>
+        <f t="shared" si="13"/>
+        <v>2039393.8480766609</v>
       </c>
       <c r="EP14" s="4">
-        <f t="shared" si="12"/>
-        <v>2796772.3301407127</v>
+        <f t="shared" si="13"/>
+        <v>2120969.6019997275</v>
       </c>
       <c r="EQ14" s="4">
-        <f t="shared" si="12"/>
-        <v>2936610.9466477484</v>
+        <f t="shared" si="13"/>
+        <v>2205808.3860797165</v>
       </c>
       <c r="ER14" s="4">
-        <f t="shared" si="12"/>
-        <v>3083441.4939801358</v>
+        <f t="shared" si="13"/>
+        <v>2294040.7215229054</v>
       </c>
       <c r="ES14" s="4">
-        <f t="shared" si="12"/>
-        <v>3237613.5686791427</v>
+        <f t="shared" si="13"/>
+        <v>2385802.3503838219</v>
       </c>
       <c r="ET14" s="4">
-        <f t="shared" si="12"/>
-        <v>3399494.2471131003</v>
+        <f t="shared" si="13"/>
+        <v>2481234.4443991748</v>
       </c>
       <c r="EU14" s="4">
-        <f t="shared" si="12"/>
-        <v>3569468.9594687554</v>
+        <f t="shared" si="13"/>
+        <v>2580483.8221751419</v>
       </c>
       <c r="EV14" s="4">
-        <f t="shared" si="12"/>
-        <v>3747942.4074421935</v>
+        <f t="shared" si="13"/>
+        <v>2683703.1750621474</v>
       </c>
       <c r="EW14" s="4">
-        <f t="shared" si="12"/>
-        <v>3935339.5278143035</v>
+        <f t="shared" si="13"/>
+        <v>2791051.3020646335</v>
       </c>
       <c r="EX14" s="4">
-        <f t="shared" si="12"/>
-        <v>4132106.5042050187</v>
+        <f t="shared" si="13"/>
+        <v>2902693.3541472191</v>
       </c>
       <c r="EY14" s="4">
-        <f t="shared" si="12"/>
-        <v>4338711.8294152701</v>
+        <f t="shared" si="13"/>
+        <v>3018801.0883131078</v>
       </c>
       <c r="EZ14" s="4">
-        <f t="shared" si="12"/>
-        <v>4555647.4208860341</v>
+        <f t="shared" si="13"/>
+        <v>3139553.1318456321</v>
       </c>
       <c r="FA14" s="4">
-        <f t="shared" si="12"/>
-        <v>4783429.7919303365</v>
+        <f t="shared" si="13"/>
+        <v>3265135.2571194577</v>
       </c>
       <c r="FB14" s="4">
-        <f t="shared" si="12"/>
-        <v>5022601.2815268533</v>
+        <f t="shared" si="13"/>
+        <v>3395740.6674042363</v>
       </c>
       <c r="FC14" s="4">
-        <f t="shared" si="12"/>
-        <v>5273731.345603196</v>
+        <f t="shared" si="13"/>
+        <v>3531570.2941004056</v>
       </c>
       <c r="FD14" s="4">
-        <f t="shared" si="12"/>
-        <v>5537417.9128833562</v>
+        <f t="shared" si="13"/>
+        <v>3672833.1058644219</v>
       </c>
       <c r="FE14" s="4">
-        <f t="shared" si="12"/>
-        <v>5814288.8085275246</v>
+        <f t="shared" si="13"/>
+        <v>3819746.4300989988</v>
       </c>
       <c r="FF14" s="4">
-        <f t="shared" si="12"/>
-        <v>6105003.2489539012</v>
+        <f t="shared" si="13"/>
+        <v>3972536.2873029588</v>
       </c>
       <c r="FG14" s="4">
-        <f t="shared" si="12"/>
-        <v>6410253.4114015969</v>
+        <f t="shared" si="13"/>
+        <v>4131437.7387950774</v>
       </c>
       <c r="FH14" s="4">
-        <f t="shared" si="12"/>
-        <v>6730766.081971677</v>
+        <f t="shared" si="13"/>
+        <v>4296695.248346881</v>
       </c>
       <c r="FI14" s="4">
-        <f t="shared" si="12"/>
-        <v>7067304.3860702608</v>
+        <f t="shared" si="13"/>
+        <v>4468563.0582807567</v>
       </c>
       <c r="FJ14" s="4">
-        <f t="shared" si="12"/>
-        <v>7420669.6053737737</v>
+        <f t="shared" si="13"/>
+        <v>4647305.580611987</v>
       </c>
       <c r="FK14" s="4">
-        <f t="shared" si="12"/>
-        <v>7791703.0856424626</v>
+        <f t="shared" si="13"/>
+        <v>4833197.8038364667</v>
       </c>
       <c r="FL14" s="4">
-        <f t="shared" si="12"/>
-        <v>8181288.2399245864</v>
+        <f t="shared" si="13"/>
+        <v>5026525.7159899259</v>
       </c>
       <c r="FM14" s="4">
-        <f t="shared" si="12"/>
-        <v>8590352.6519208159</v>
+        <f t="shared" si="13"/>
+        <v>5227586.7446295228</v>
       </c>
       <c r="FN14" s="4">
-        <f t="shared" si="12"/>
-        <v>9019870.2845168579</v>
+        <f t="shared" si="13"/>
+        <v>5436690.2144147037</v>
       </c>
       <c r="FO14" s="4">
-        <f t="shared" si="12"/>
-        <v>9470863.7987427004</v>
+        <f t="shared" si="13"/>
+        <v>5654157.822991292</v>
       </c>
       <c r="FP14" s="4">
-        <f t="shared" si="12"/>
-        <v>9944406.9886798356</v>
+        <f t="shared" si="13"/>
+        <v>5880324.1359109441</v>
       </c>
       <c r="FQ14" s="4">
-        <f t="shared" si="12"/>
-        <v>10441627.338113828</v>
+        <f t="shared" si="13"/>
+        <v>6115537.1013473822</v>
       </c>
       <c r="FR14" s="4">
-        <f t="shared" si="12"/>
-        <v>10963708.705019519</v>
+        <f t="shared" ref="FR14:FV14" si="14">FQ14*($AD5+1)</f>
+        <v>6360158.585401278</v>
       </c>
       <c r="FS14" s="4">
-        <f t="shared" si="12"/>
-        <v>11511894.140270496</v>
+        <f t="shared" si="14"/>
+        <v>6614564.928817329</v>
       </c>
       <c r="FT14" s="4">
-        <f t="shared" si="12"/>
-        <v>12087488.847284021</v>
+        <f t="shared" si="14"/>
+        <v>6879147.5259700222</v>
       </c>
       <c r="FU14" s="4">
-        <f t="shared" si="12"/>
-        <v>12691863.289648222</v>
+        <f t="shared" si="14"/>
+        <v>7154313.4270088235</v>
       </c>
       <c r="FV14" s="4">
-        <f t="shared" si="12"/>
-        <v>13326456.454130633</v>
-      </c>
-      <c r="FW14" s="4">
-        <f t="shared" ref="FW14:GA14" si="13">FV14*($AD5+1)</f>
-        <v>13992779.276837165</v>
-      </c>
-      <c r="FX14" s="4">
-        <f t="shared" si="13"/>
-        <v>14692418.240679024</v>
-      </c>
-      <c r="FY14" s="4">
-        <f t="shared" si="13"/>
-        <v>15427039.152712977</v>
-      </c>
-      <c r="FZ14" s="4">
-        <f t="shared" si="13"/>
-        <v>16198391.110348627</v>
-      </c>
-      <c r="GA14" s="4">
-        <f t="shared" si="13"/>
-        <v>17008310.665866058</v>
+        <f t="shared" si="14"/>
+        <v>7440485.9640891766</v>
       </c>
     </row>
-    <row r="15" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
-      <c r="AG15" s="4"/>
-      <c r="AH15" s="4"/>
-      <c r="AI15" s="4"/>
-      <c r="AJ15" s="1"/>
-      <c r="AK15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL15" s="4">
-        <v>4117</v>
-      </c>
-      <c r="AM15" s="4">
-        <v>3764</v>
-      </c>
-      <c r="AN15" s="4">
-        <v>5418</v>
-      </c>
-      <c r="AO15" s="4">
-        <v>9166</v>
-      </c>
-      <c r="AP15" s="4">
-        <v>13001</v>
-      </c>
-      <c r="AQ15" s="4">
-        <v>16181</v>
-      </c>
-      <c r="AR15" s="4">
-        <v>22112</v>
-      </c>
-      <c r="AS15" s="4">
-        <v>18485</v>
-      </c>
-      <c r="AT15" s="4">
-        <v>29082</v>
-      </c>
-      <c r="AU15" s="4">
-        <v>39370</v>
-      </c>
-      <c r="AV15" s="4">
-        <v>23448</v>
-      </c>
-      <c r="AW15" s="4">
-        <f>AV15*($AG5+1)</f>
-        <v>24327.300000000003</v>
-      </c>
-      <c r="AX15" s="4">
-        <f t="shared" ref="AX15:DI15" si="14">AW15*($AG5+1)</f>
-        <v>25239.573750000007</v>
-      </c>
-      <c r="AY15" s="4">
-        <f t="shared" si="14"/>
-        <v>26186.05776562501</v>
-      </c>
-      <c r="AZ15" s="4">
-        <f t="shared" si="14"/>
-        <v>27168.034931835951</v>
-      </c>
-      <c r="BA15" s="4">
-        <f t="shared" si="14"/>
-        <v>28186.836241779802</v>
-      </c>
-      <c r="BB15" s="4">
-        <f t="shared" si="14"/>
-        <v>29243.842600846547</v>
-      </c>
-      <c r="BC15" s="4">
-        <f t="shared" si="14"/>
-        <v>30340.486698378296</v>
-      </c>
-      <c r="BD15" s="4">
-        <f t="shared" si="14"/>
-        <v>31478.254949567483</v>
-      </c>
-      <c r="BE15" s="4">
-        <f t="shared" si="14"/>
-        <v>32658.689510176268</v>
-      </c>
-      <c r="BF15" s="4">
-        <f t="shared" si="14"/>
-        <v>33883.390366807878</v>
-      </c>
-      <c r="BG15" s="4">
-        <f t="shared" si="14"/>
-        <v>35154.017505563177</v>
-      </c>
-      <c r="BH15" s="4">
-        <f t="shared" si="14"/>
-        <v>36472.293162021801</v>
-      </c>
-      <c r="BI15" s="4">
-        <f t="shared" si="14"/>
-        <v>37840.00415559762</v>
-      </c>
-      <c r="BJ15" s="4">
-        <f t="shared" si="14"/>
-        <v>39259.004311432538</v>
-      </c>
-      <c r="BK15" s="4">
-        <f t="shared" si="14"/>
-        <v>40731.216973111259</v>
-      </c>
-      <c r="BL15" s="4">
-        <f t="shared" si="14"/>
-        <v>42258.637609602934</v>
-      </c>
-      <c r="BM15" s="4">
-        <f t="shared" si="14"/>
-        <v>43843.33651996305</v>
-      </c>
-      <c r="BN15" s="4">
-        <f t="shared" si="14"/>
-        <v>45487.461639461668</v>
-      </c>
-      <c r="BO15" s="4">
-        <f t="shared" si="14"/>
-        <v>47193.241450941481</v>
-      </c>
-      <c r="BP15" s="4">
-        <f t="shared" si="14"/>
-        <v>48962.988005351792</v>
-      </c>
-      <c r="BQ15" s="4">
-        <f t="shared" si="14"/>
-        <v>50799.100055552488</v>
-      </c>
-      <c r="BR15" s="4">
-        <f t="shared" si="14"/>
-        <v>52704.066307635709</v>
-      </c>
-      <c r="BS15" s="4">
-        <f t="shared" si="14"/>
-        <v>54680.468794172055</v>
-      </c>
-      <c r="BT15" s="4">
-        <f t="shared" si="14"/>
-        <v>56730.986373953514</v>
-      </c>
-      <c r="BU15" s="4">
-        <f t="shared" si="14"/>
-        <v>58858.398362976775</v>
-      </c>
-      <c r="BV15" s="4">
-        <f t="shared" si="14"/>
-        <v>61065.58830158841</v>
-      </c>
-      <c r="BW15" s="4">
-        <f t="shared" si="14"/>
-        <v>63355.547862897984</v>
-      </c>
-      <c r="BX15" s="4">
-        <f t="shared" si="14"/>
-        <v>65731.380907756669</v>
-      </c>
-      <c r="BY15" s="4">
-        <f t="shared" si="14"/>
-        <v>68196.307691797556</v>
-      </c>
-      <c r="BZ15" s="4">
-        <f t="shared" si="14"/>
-        <v>70753.669230239975</v>
-      </c>
-      <c r="CA15" s="4">
-        <f t="shared" si="14"/>
-        <v>73406.931826373984</v>
-      </c>
-      <c r="CB15" s="4">
-        <f t="shared" si="14"/>
-        <v>76159.691769863013</v>
-      </c>
-      <c r="CC15" s="4">
-        <f t="shared" si="14"/>
-        <v>79015.680211232888</v>
-      </c>
-      <c r="CD15" s="4">
-        <f t="shared" si="14"/>
-        <v>81978.768219154124</v>
-      </c>
-      <c r="CE15" s="4">
-        <f t="shared" si="14"/>
-        <v>85052.972027372409</v>
-      </c>
-      <c r="CF15" s="4">
-        <f t="shared" si="14"/>
-        <v>88242.458478398883</v>
-      </c>
-      <c r="CG15" s="4">
-        <f t="shared" si="14"/>
-        <v>91551.550671338846</v>
-      </c>
-      <c r="CH15" s="4">
-        <f t="shared" si="14"/>
-        <v>94984.733821514063</v>
-      </c>
-      <c r="CI15" s="4">
-        <f t="shared" si="14"/>
-        <v>98546.661339820843</v>
-      </c>
-      <c r="CJ15" s="4">
-        <f t="shared" si="14"/>
-        <v>102242.16114006413</v>
-      </c>
-      <c r="CK15" s="4">
-        <f t="shared" si="14"/>
-        <v>106076.24218281654</v>
-      </c>
-      <c r="CL15" s="4">
-        <f t="shared" si="14"/>
-        <v>110054.10126467216</v>
-      </c>
-      <c r="CM15" s="4">
-        <f t="shared" si="14"/>
-        <v>114181.13006209738</v>
-      </c>
-      <c r="CN15" s="4">
-        <f t="shared" si="14"/>
-        <v>118462.92243942604</v>
-      </c>
-      <c r="CO15" s="4">
-        <f t="shared" si="14"/>
-        <v>122905.28203090452</v>
-      </c>
-      <c r="CP15" s="4">
-        <f t="shared" si="14"/>
-        <v>127514.23010706346</v>
-      </c>
-      <c r="CQ15" s="4">
-        <f t="shared" si="14"/>
-        <v>132296.01373607834</v>
-      </c>
-      <c r="CR15" s="4">
-        <f t="shared" si="14"/>
-        <v>137257.11425118128</v>
-      </c>
-      <c r="CS15" s="4">
-        <f t="shared" si="14"/>
-        <v>142404.25603560059</v>
-      </c>
-      <c r="CT15" s="4">
-        <f t="shared" si="14"/>
-        <v>147744.41563693562</v>
-      </c>
-      <c r="CU15" s="4">
-        <f t="shared" si="14"/>
-        <v>153284.83122332071</v>
-      </c>
-      <c r="CV15" s="4">
-        <f t="shared" si="14"/>
-        <v>159033.01239419525</v>
-      </c>
-      <c r="CW15" s="4">
-        <f t="shared" si="14"/>
-        <v>164996.75035897759</v>
-      </c>
-      <c r="CX15" s="4">
-        <f t="shared" si="14"/>
-        <v>171184.12849743926</v>
-      </c>
-      <c r="CY15" s="4">
-        <f t="shared" si="14"/>
-        <v>177603.53331609324</v>
-      </c>
-      <c r="CZ15" s="4">
-        <f t="shared" si="14"/>
-        <v>184263.66581544676</v>
-      </c>
-      <c r="DA15" s="4">
-        <f t="shared" si="14"/>
-        <v>191173.55328352604</v>
-      </c>
-      <c r="DB15" s="4">
-        <f t="shared" si="14"/>
-        <v>198342.56153165828</v>
-      </c>
-      <c r="DC15" s="4">
-        <f t="shared" si="14"/>
-        <v>205780.4075890955</v>
-      </c>
-      <c r="DD15" s="4">
-        <f t="shared" si="14"/>
-        <v>213497.17287368659</v>
-      </c>
-      <c r="DE15" s="4">
-        <f t="shared" si="14"/>
-        <v>221503.31685644985</v>
-      </c>
-      <c r="DF15" s="4">
-        <f t="shared" si="14"/>
-        <v>229809.69123856674</v>
-      </c>
-      <c r="DG15" s="4">
-        <f t="shared" si="14"/>
-        <v>238427.554660013</v>
-      </c>
-      <c r="DH15" s="4">
-        <f t="shared" si="14"/>
-        <v>247368.58795976351</v>
-      </c>
-      <c r="DI15" s="4">
-        <f t="shared" si="14"/>
-        <v>256644.91000825466</v>
-      </c>
-      <c r="DJ15" s="4">
-        <f t="shared" ref="DJ15:FU15" si="15">DI15*($AG5+1)</f>
-        <v>266269.09413356421</v>
-      </c>
-      <c r="DK15" s="4">
-        <f t="shared" si="15"/>
-        <v>276254.1851635729</v>
-      </c>
-      <c r="DL15" s="4">
-        <f t="shared" si="15"/>
-        <v>286613.71710720693</v>
-      </c>
-      <c r="DM15" s="4">
-        <f t="shared" si="15"/>
-        <v>297361.73149872723</v>
-      </c>
-      <c r="DN15" s="4">
-        <f t="shared" si="15"/>
-        <v>308512.7964299295</v>
-      </c>
-      <c r="DO15" s="4">
-        <f t="shared" si="15"/>
-        <v>320082.02629605186</v>
-      </c>
-      <c r="DP15" s="4">
-        <f t="shared" si="15"/>
-        <v>332085.10228215385</v>
-      </c>
-      <c r="DQ15" s="4">
-        <f t="shared" si="15"/>
-        <v>344538.29361773463</v>
-      </c>
-      <c r="DR15" s="4">
-        <f t="shared" si="15"/>
-        <v>357458.47962839971</v>
-      </c>
-      <c r="DS15" s="4">
-        <f t="shared" si="15"/>
-        <v>370863.17261446471</v>
-      </c>
-      <c r="DT15" s="4">
-        <f t="shared" si="15"/>
-        <v>384770.54158750718</v>
-      </c>
-      <c r="DU15" s="4">
-        <f t="shared" si="15"/>
-        <v>399199.43689703871</v>
-      </c>
-      <c r="DV15" s="4">
-        <f t="shared" si="15"/>
-        <v>414169.41578067769</v>
-      </c>
-      <c r="DW15" s="4">
-        <f t="shared" si="15"/>
-        <v>429700.76887245313</v>
-      </c>
-      <c r="DX15" s="4">
-        <f t="shared" si="15"/>
-        <v>445814.54770517017</v>
-      </c>
-      <c r="DY15" s="4">
-        <f t="shared" si="15"/>
-        <v>462532.59324411408</v>
-      </c>
-      <c r="DZ15" s="4">
-        <f t="shared" si="15"/>
-        <v>479877.56549076841</v>
-      </c>
-      <c r="EA15" s="4">
-        <f t="shared" si="15"/>
-        <v>497872.97419667226</v>
-      </c>
-      <c r="EB15" s="4">
-        <f t="shared" si="15"/>
-        <v>516543.21072904754</v>
-      </c>
-      <c r="EC15" s="4">
-        <f t="shared" si="15"/>
-        <v>535913.58113138692</v>
-      </c>
-      <c r="ED15" s="4">
-        <f t="shared" si="15"/>
-        <v>556010.34042381402</v>
-      </c>
-      <c r="EE15" s="4">
-        <f t="shared" si="15"/>
-        <v>576860.72818970715</v>
-      </c>
-      <c r="EF15" s="4">
-        <f t="shared" si="15"/>
-        <v>598493.00549682125</v>
-      </c>
-      <c r="EG15" s="4">
-        <f t="shared" si="15"/>
-        <v>620936.49320295209</v>
-      </c>
-      <c r="EH15" s="4">
-        <f t="shared" si="15"/>
-        <v>644221.61169806286</v>
-      </c>
-      <c r="EI15" s="4">
-        <f t="shared" si="15"/>
-        <v>668379.92213674029</v>
-      </c>
-      <c r="EJ15" s="4">
-        <f t="shared" si="15"/>
-        <v>693444.16921686812</v>
-      </c>
-      <c r="EK15" s="4">
-        <f t="shared" si="15"/>
-        <v>719448.32556250074</v>
-      </c>
-      <c r="EL15" s="4">
-        <f t="shared" si="15"/>
-        <v>746427.63777109457</v>
-      </c>
-      <c r="EM15" s="4">
-        <f t="shared" si="15"/>
-        <v>774418.67418751062</v>
-      </c>
-      <c r="EN15" s="4">
-        <f t="shared" si="15"/>
-        <v>803459.37446954229</v>
-      </c>
-      <c r="EO15" s="4">
-        <f t="shared" si="15"/>
-        <v>833589.10101215017</v>
-      </c>
-      <c r="EP15" s="4">
-        <f t="shared" si="15"/>
-        <v>864848.69230010593</v>
-      </c>
-      <c r="EQ15" s="4">
-        <f t="shared" si="15"/>
-        <v>897280.51826136</v>
-      </c>
-      <c r="ER15" s="4">
-        <f t="shared" si="15"/>
-        <v>930928.53769616107</v>
-      </c>
-      <c r="ES15" s="4">
-        <f t="shared" si="15"/>
-        <v>965838.35785976716</v>
-      </c>
-      <c r="ET15" s="4">
-        <f t="shared" si="15"/>
-        <v>1002057.2962795085</v>
-      </c>
-      <c r="EU15" s="4">
-        <f t="shared" si="15"/>
-        <v>1039634.4448899901</v>
-      </c>
-      <c r="EV15" s="4">
-        <f t="shared" si="15"/>
-        <v>1078620.7365733648</v>
-      </c>
-      <c r="EW15" s="4">
-        <f t="shared" si="15"/>
-        <v>1119069.0141948662</v>
-      </c>
-      <c r="EX15" s="4">
-        <f t="shared" si="15"/>
-        <v>1161034.1022271737</v>
-      </c>
-      <c r="EY15" s="4">
-        <f t="shared" si="15"/>
-        <v>1204572.8810606929</v>
-      </c>
-      <c r="EZ15" s="4">
-        <f t="shared" si="15"/>
-        <v>1249744.364100469</v>
-      </c>
-      <c r="FA15" s="4">
-        <f t="shared" si="15"/>
-        <v>1296609.7777542367</v>
-      </c>
-      <c r="FB15" s="4">
-        <f t="shared" si="15"/>
-        <v>1345232.6444200207</v>
-      </c>
-      <c r="FC15" s="4">
-        <f t="shared" si="15"/>
-        <v>1395678.8685857716</v>
-      </c>
-      <c r="FD15" s="4">
-        <f t="shared" si="15"/>
-        <v>1448016.8261577382</v>
-      </c>
-      <c r="FE15" s="4">
-        <f t="shared" si="15"/>
-        <v>1502317.4571386536</v>
-      </c>
-      <c r="FF15" s="4">
-        <f t="shared" si="15"/>
-        <v>1558654.3617813534</v>
-      </c>
-      <c r="FG15" s="4">
-        <f t="shared" si="15"/>
-        <v>1617103.9003481544</v>
-      </c>
-      <c r="FH15" s="4">
-        <f t="shared" si="15"/>
-        <v>1677745.2966112103</v>
-      </c>
-      <c r="FI15" s="4">
-        <f t="shared" si="15"/>
-        <v>1740660.7452341309</v>
-      </c>
-      <c r="FJ15" s="4">
-        <f t="shared" si="15"/>
-        <v>1805935.523180411</v>
-      </c>
-      <c r="FK15" s="4">
-        <f t="shared" si="15"/>
-        <v>1873658.1052996765</v>
-      </c>
-      <c r="FL15" s="4">
-        <f t="shared" si="15"/>
-        <v>1943920.2842484147</v>
-      </c>
-      <c r="FM15" s="4">
-        <f t="shared" si="15"/>
-        <v>2016817.2949077303</v>
-      </c>
-      <c r="FN15" s="4">
-        <f t="shared" si="15"/>
-        <v>2092447.9434667705</v>
-      </c>
-      <c r="FO15" s="4">
-        <f t="shared" si="15"/>
-        <v>2170914.7413467746</v>
-      </c>
-      <c r="FP15" s="4">
-        <f t="shared" si="15"/>
-        <v>2252324.0441472786</v>
-      </c>
-      <c r="FQ15" s="4">
-        <f t="shared" si="15"/>
-        <v>2336786.1958028018</v>
-      </c>
-      <c r="FR15" s="4">
-        <f t="shared" si="15"/>
-        <v>2424415.6781454072</v>
-      </c>
-      <c r="FS15" s="4">
-        <f t="shared" si="15"/>
-        <v>2515331.2660758602</v>
-      </c>
-      <c r="FT15" s="4">
-        <f t="shared" si="15"/>
-        <v>2609656.1885537053</v>
-      </c>
-      <c r="FU15" s="4">
-        <f t="shared" si="15"/>
-        <v>2707518.2956244694</v>
-      </c>
-      <c r="FV15" s="4">
-        <f t="shared" ref="FV15:GA15" si="16">FU15*($AG5+1)</f>
-        <v>2809050.2317103874</v>
-      </c>
-      <c r="FW15" s="4">
-        <f t="shared" si="16"/>
-        <v>2914389.6153995274</v>
-      </c>
-      <c r="FX15" s="4">
-        <f t="shared" si="16"/>
-        <v>3023679.2259770101</v>
-      </c>
-      <c r="FY15" s="4">
-        <f t="shared" si="16"/>
-        <v>3137067.1969511481</v>
-      </c>
-      <c r="FZ15" s="4">
-        <f t="shared" si="16"/>
-        <v>3254707.2168368166</v>
-      </c>
-      <c r="GA15" s="4">
-        <f t="shared" si="16"/>
-        <v>3376758.7374681975</v>
-      </c>
+    <row r="15" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="AM15" s="4"/>
     </row>
-    <row r="16" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="AR16" s="4"/>
-    </row>
-    <row r="17" spans="3:79" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+    <row r="16" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D17">
+      <c r="D16">
         <v>1.69</v>
       </c>
-      <c r="E17">
+      <c r="E16">
         <v>1.74</v>
       </c>
-      <c r="F17">
+      <c r="F16">
         <v>1.76</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G16" s="9">
         <f>7.57/4</f>
         <v>1.8925000000000001</v>
       </c>
-      <c r="H17">
+      <c r="H16">
         <v>0.85</v>
       </c>
-      <c r="I17">
+      <c r="I16">
         <v>0.91</v>
       </c>
-      <c r="J17">
+      <c r="J16">
         <v>2.12</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K16" s="9">
         <f>6.43/4</f>
         <v>1.6074999999999999</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L16" s="9">
         <v>1.71</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M16" s="9">
         <v>1.8</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N16" s="9">
         <v>2.71</v>
       </c>
-      <c r="O17" s="9">
+      <c r="O16" s="9">
         <f>10.09/4</f>
         <v>2.5225</v>
       </c>
-      <c r="P17" s="9">
+      <c r="P16" s="9">
         <v>3.3</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="Q16" s="9">
         <v>3.61</v>
       </c>
-      <c r="R17" s="9">
+      <c r="R16" s="9">
         <v>3.22</v>
       </c>
-      <c r="S17" s="9">
+      <c r="S16" s="9">
         <f>13.77/4</f>
         <v>3.4424999999999999</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T16" s="9">
         <v>2.72</v>
       </c>
-      <c r="U17" s="9">
+      <c r="U16" s="9">
         <v>2.46</v>
       </c>
-      <c r="V17" s="9">
+      <c r="V16" s="9">
         <v>1.64</v>
       </c>
-      <c r="W17" s="9">
+      <c r="W16" s="9">
         <f>8.59/4</f>
         <v>2.1475</v>
       </c>
-      <c r="X17" s="9">
+      <c r="X16" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Y17" s="9">
+      <c r="Y16" s="9">
         <v>2.98</v>
       </c>
-      <c r="Z17" s="9">
+      <c r="Z16" s="9">
         <v>2.5</v>
       </c>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="9"/>
-      <c r="AI17" s="9"/>
-      <c r="AJ17" s="1"/>
-      <c r="AK17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL17" s="9">
+      <c r="AA16" s="9">
+        <v>5.33</v>
+      </c>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="9">
         <v>0.01</v>
       </c>
-      <c r="AM17" s="9">
+      <c r="AH16" s="9">
         <v>0.6</v>
       </c>
-      <c r="AN17" s="9">
+      <c r="AI16" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AO17" s="9">
+      <c r="AJ16" s="9">
         <v>1.29</v>
       </c>
-      <c r="AP17" s="9">
+      <c r="AK16" s="9">
         <v>3.49</v>
       </c>
-      <c r="AQ17" s="9">
+      <c r="AL16" s="9">
         <v>5.39</v>
       </c>
-      <c r="AR17" s="9">
-        <f>SUM(D17:G17)</f>
+      <c r="AM16" s="9">
+        <f>SUM(D16:G16)</f>
         <v>7.0824999999999996</v>
       </c>
-      <c r="AS17" s="9">
-        <f>SUM(H17:K17)</f>
+      <c r="AN16" s="9">
+        <f>SUM(H16:K16)</f>
         <v>5.4874999999999998</v>
       </c>
-      <c r="AT17" s="9">
-        <f>SUM(O17:R17)</f>
+      <c r="AO16" s="9">
+        <f>SUM(O16:R16)</f>
         <v>12.6525</v>
       </c>
-      <c r="AU17" s="9">
-        <f>SUM(S17:W17)</f>
+      <c r="AP16" s="9">
+        <f>SUM(S16:W16)</f>
         <v>12.41</v>
       </c>
-      <c r="AV17" s="9">
-        <f>SUM(T17:W17)</f>
+      <c r="AQ16" s="9">
+        <f>SUM(T16:W16)</f>
         <v>8.9674999999999994</v>
       </c>
-      <c r="AW17" s="9"/>
-      <c r="AX17" s="9"/>
-      <c r="AY17" s="9"/>
-      <c r="AZ17" s="9"/>
-      <c r="BA17" s="9"/>
-      <c r="BB17" s="9"/>
-      <c r="BC17" s="9"/>
-      <c r="BD17" s="9"/>
-      <c r="BE17" s="9"/>
-      <c r="BF17" s="9"/>
-      <c r="BG17" s="9"/>
-      <c r="BH17" s="9"/>
-      <c r="BI17" s="9"/>
-      <c r="BJ17" s="9"/>
-      <c r="BK17" s="9"/>
-      <c r="BL17" s="9"/>
-      <c r="BM17" s="9"/>
-      <c r="BN17" s="9"/>
+      <c r="AR16" s="9">
+        <f>SUM(X16:AA16)</f>
+        <v>13.01</v>
+      </c>
+      <c r="AS16" s="9"/>
+      <c r="AT16" s="9"/>
+      <c r="AU16" s="9"/>
+      <c r="AV16" s="9"/>
+      <c r="AW16" s="9"/>
+      <c r="AX16" s="9"/>
+      <c r="AY16" s="9"/>
+      <c r="AZ16" s="9"/>
+      <c r="BA16" s="9"/>
+      <c r="BB16" s="9"/>
+      <c r="BC16" s="9"/>
+      <c r="BD16" s="9"/>
+      <c r="BE16" s="9"/>
+      <c r="BF16" s="9"/>
+      <c r="BG16" s="9"/>
+      <c r="BH16" s="9"/>
+      <c r="BI16" s="9"/>
     </row>
-    <row r="18" spans="3:79" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
+    <row r="17" spans="3:74" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D17" s="4">
         <v>2945</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E17" s="4">
         <v>2930</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F17" s="4">
         <v>2913</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G17" s="4">
         <v>2921</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H17" s="4">
         <v>2869</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I17" s="4">
         <v>2875</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J17" s="4">
         <v>2874</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K17" s="4">
         <v>2876</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L17" s="4">
         <v>2868</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M17" s="4">
         <v>2879</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N17" s="4">
         <v>2891</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O17" s="4">
         <v>2888</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P17" s="4">
         <v>2882</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q17" s="4">
         <v>2877</v>
       </c>
-      <c r="R18" s="4">
+      <c r="R17" s="4">
         <v>2859</v>
       </c>
-      <c r="S18" s="4">
+      <c r="S17" s="4">
         <v>2859</v>
       </c>
-      <c r="T18" s="4">
+      <c r="T17" s="4">
         <v>2742</v>
       </c>
-      <c r="U18" s="4">
+      <c r="U17" s="4">
         <v>2713</v>
       </c>
-      <c r="V18" s="4">
+      <c r="V17" s="4">
         <v>2687</v>
       </c>
-      <c r="W18" s="4">
+      <c r="W17" s="4">
         <f>2702</f>
         <v>2702</v>
       </c>
-      <c r="X18" s="4">
+      <c r="X17" s="4">
         <v>2596</v>
       </c>
-      <c r="Y18" s="4">
+      <c r="Y17" s="4">
         <v>2612</v>
       </c>
-      <c r="Z18" s="4">
+      <c r="Z17" s="4">
         <v>2576</v>
       </c>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="4"/>
-      <c r="AF18" s="4"/>
-      <c r="AG18" s="4"/>
-      <c r="AH18" s="4"/>
-      <c r="AI18" s="4"/>
-      <c r="AJ18" s="1"/>
-      <c r="AK18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL18" s="4">
+      <c r="AA17" s="4">
+        <v>2630</v>
+      </c>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="4">
         <v>2166</v>
       </c>
-      <c r="AM18" s="4">
+      <c r="AH17" s="4">
         <v>2517</v>
       </c>
-      <c r="AN18" s="4">
+      <c r="AI17" s="4">
         <v>2664</v>
       </c>
-      <c r="AO18" s="4">
+      <c r="AJ17" s="4">
         <v>2853</v>
       </c>
-      <c r="AP18" s="4">
+      <c r="AK17" s="4">
         <v>2925</v>
       </c>
-      <c r="AQ18" s="4">
+      <c r="AL17" s="4">
         <v>2956</v>
       </c>
-      <c r="AR18" s="4">
+      <c r="AM17" s="4">
         <v>2921</v>
       </c>
-      <c r="AS18" s="4">
+      <c r="AN17" s="4">
         <v>2876</v>
       </c>
-      <c r="AT18" s="4">
+      <c r="AO17" s="4">
         <v>2888</v>
       </c>
-      <c r="AU18" s="4">
+      <c r="AP17" s="4">
         <v>2859</v>
       </c>
-      <c r="AV18" s="4">
+      <c r="AQ17" s="4">
         <f>2702</f>
         <v>2702</v>
       </c>
-      <c r="AW18" s="4"/>
-      <c r="AX18" s="4"/>
-      <c r="AY18" s="4"/>
-      <c r="AZ18" s="4"/>
-      <c r="BA18" s="4"/>
-      <c r="BB18" s="4"/>
-      <c r="BC18" s="4"/>
-      <c r="BD18" s="4"/>
-      <c r="BE18" s="4"/>
-      <c r="BF18" s="4"/>
-      <c r="BG18" s="4"/>
-      <c r="BH18" s="4"/>
-      <c r="BI18" s="4"/>
-      <c r="BJ18" s="4"/>
-      <c r="BK18" s="4"/>
-      <c r="BL18" s="4"/>
-      <c r="BM18" s="4"/>
-      <c r="BN18" s="4"/>
-      <c r="BO18" s="4"/>
-      <c r="BP18" s="4"/>
-      <c r="BQ18" s="4"/>
-      <c r="BR18" s="4"/>
-      <c r="BS18" s="4"/>
-      <c r="BT18" s="4"/>
-      <c r="BU18" s="4"/>
-      <c r="BV18" s="4"/>
-      <c r="BW18" s="4"/>
-      <c r="BX18" s="4"/>
-      <c r="BY18" s="4"/>
-      <c r="BZ18" s="4"/>
-      <c r="CA18" s="4"/>
+      <c r="AR17" s="4">
+        <v>2630</v>
+      </c>
+      <c r="AS17" s="4"/>
+      <c r="AT17" s="4"/>
+      <c r="AU17" s="4"/>
+      <c r="AV17" s="4"/>
+      <c r="AW17" s="4"/>
+      <c r="AX17" s="4"/>
+      <c r="AY17" s="4"/>
+      <c r="AZ17" s="4"/>
+      <c r="BA17" s="4"/>
+      <c r="BB17" s="4"/>
+      <c r="BC17" s="4"/>
+      <c r="BD17" s="4"/>
+      <c r="BE17" s="4"/>
+      <c r="BF17" s="4"/>
+      <c r="BG17" s="4"/>
+      <c r="BH17" s="4"/>
+      <c r="BI17" s="4"/>
+      <c r="BJ17" s="4"/>
+      <c r="BK17" s="4"/>
+      <c r="BL17" s="4"/>
+      <c r="BM17" s="4"/>
+      <c r="BN17" s="4"/>
+      <c r="BO17" s="4"/>
+      <c r="BP17" s="4"/>
+      <c r="BQ17" s="4"/>
+      <c r="BR17" s="4"/>
+      <c r="BS17" s="4"/>
+      <c r="BT17" s="4"/>
+      <c r="BU17" s="4"/>
+      <c r="BV17" s="4"/>
     </row>
-    <row r="20" spans="3:79" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:74" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10">
+        <f>E5/D5-1</f>
+        <v>0.10571619588835035</v>
+      </c>
+      <c r="F19" s="10">
+        <f>F5/E5-1</f>
+        <v>3.7487718237472656E-2</v>
+      </c>
+      <c r="G19" s="10">
+        <f>G5/F5-1</f>
+        <v>0.23217017556640207</v>
+      </c>
+      <c r="H19" s="10">
+        <f>H5/G5-1</f>
+        <v>-0.10860825351779591</v>
+      </c>
+      <c r="I19" s="10">
+        <f>I5/H5-1</f>
+        <v>0.11998408171386887</v>
+      </c>
+      <c r="J19" s="10">
+        <f>J5/I5-1</f>
+        <v>4.536302262229075E-2</v>
+      </c>
+      <c r="K19" s="10">
+        <f>K5/J5-1</f>
+        <v>0.19431225923408113</v>
+      </c>
+      <c r="L19" s="10">
+        <f>L5/K5-1</f>
+        <v>-0.15866616070581541</v>
+      </c>
+      <c r="M19" s="10">
+        <f>M5/L5-1</f>
+        <v>5.3560354062130111E-2</v>
+      </c>
+      <c r="N19" s="10">
+        <f>N5/M5-1</f>
+        <v>0.14892706159362112</v>
+      </c>
+      <c r="O19" s="10">
+        <f>O5/N5-1</f>
+        <v>0.30745225896599915</v>
+      </c>
+      <c r="P19" s="10">
+        <f>P5/O5-1</f>
+        <v>-6.7685511738092674E-2</v>
+      </c>
+      <c r="Q19" s="10">
+        <f>Q5/P5-1</f>
+        <v>0.11103893622712158</v>
+      </c>
+      <c r="R19" s="10">
+        <f>R5/Q5-1</f>
+        <v>-2.3042267083949186E-3</v>
+      </c>
+      <c r="S19" s="10">
+        <f>S5/R5-1</f>
+        <v>0.16066873491899347</v>
+      </c>
+      <c r="T19" s="10">
+        <f>T5/S5-1</f>
+        <v>-0.1711561878174096</v>
+      </c>
+      <c r="U19" s="10">
+        <f>U5/T5-1</f>
+        <v>3.2750465816253405E-2</v>
+      </c>
+      <c r="V19" s="10">
+        <f>V5/U5-1</f>
+        <v>-3.8442856151550853E-2</v>
+      </c>
+      <c r="W19" s="10">
+        <f>W5/V5-1</f>
+        <v>0.1606047485025619</v>
+      </c>
+      <c r="X19" s="10">
+        <f>X5/W5-1</f>
+        <v>-0.10943572205813767</v>
+      </c>
+      <c r="Y19" s="10">
+        <f>Y5/X5-1</f>
+        <v>0.1170884971199162</v>
+      </c>
+      <c r="Z19" s="10">
+        <f>Z5/Y5-1</f>
+        <v>6.7095846745210741E-2</v>
+      </c>
+      <c r="AA19" s="10">
+        <f>AA5/Z5-1</f>
+        <v>0.17469103262461205</v>
+      </c>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="10"/>
+      <c r="AH19" s="10">
+        <f>AH5/AG5-1</f>
+        <v>0.5468657889565729</v>
+      </c>
+      <c r="AI19" s="10">
+        <f t="shared" ref="AI19:AR19" si="15">AI5/AH5-1</f>
+        <v>0.58358739837398366</v>
+      </c>
+      <c r="AJ19" s="10">
+        <f t="shared" si="15"/>
+        <v>0.43815177282207607</v>
+      </c>
+      <c r="AK19" s="10">
+        <f t="shared" si="15"/>
+        <v>0.54161088799643009</v>
+      </c>
+      <c r="AL19" s="10">
+        <f t="shared" si="15"/>
+        <v>0.47090961719371882</v>
+      </c>
+      <c r="AM19" s="10">
+        <f t="shared" si="15"/>
+        <v>0.37352716896661997</v>
+      </c>
+      <c r="AN19" s="10">
+        <f t="shared" si="15"/>
+        <v>0.26610910132884413</v>
+      </c>
+      <c r="AO19" s="10">
+        <f t="shared" si="15"/>
+        <v>0.21596390228722573</v>
+      </c>
+      <c r="AP19" s="10">
+        <f t="shared" si="15"/>
+        <v>0.37182574303495608</v>
+      </c>
+      <c r="AQ19" s="10">
+        <f t="shared" si="15"/>
+        <v>-1.1193175554782941E-2</v>
+      </c>
+      <c r="AR19" s="10">
+        <f t="shared" si="15"/>
+        <v>0.15686610810486323</v>
+      </c>
+      <c r="AS19" s="10"/>
+      <c r="AT19" s="10"/>
+      <c r="AU19" s="10"/>
+      <c r="AV19" s="10"/>
+      <c r="AW19" s="10"/>
+      <c r="AX19" s="10"/>
+      <c r="AY19" s="10"/>
+      <c r="AZ19" s="10"/>
+      <c r="BA19" s="10"/>
+      <c r="BB19" s="10"/>
+      <c r="BC19" s="10"/>
+      <c r="BD19" s="10"/>
+      <c r="BE19" s="10"/>
+      <c r="BF19" s="10"/>
+      <c r="BG19" s="10"/>
+      <c r="BH19" s="10"/>
+      <c r="BI19" s="10"/>
+      <c r="BJ19" s="10"/>
+      <c r="BK19" s="10"/>
+      <c r="BL19" s="10"/>
+      <c r="BM19" s="10"/>
+      <c r="BN19" s="10"/>
+      <c r="BO19" s="10"/>
+      <c r="BP19" s="10"/>
+      <c r="BQ19" s="10"/>
+      <c r="BR19" s="10"/>
+      <c r="BS19" s="10"/>
+      <c r="BT19" s="10"/>
+      <c r="BU19" s="10"/>
+    </row>
+    <row r="20" spans="3:74" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10">
-        <f>E5/D5-1</f>
-        <v>0.10571619588835035</v>
+        <f>E14/D14-1</f>
+        <v>2.3656776263031309E-2</v>
       </c>
       <c r="F20" s="10">
-        <f t="shared" ref="F20:Z20" si="17">F5/E5-1</f>
-        <v>3.7487718237472656E-2</v>
+        <f>F14/E14-1</f>
+        <v>6.0712886799842991E-3</v>
       </c>
       <c r="G20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.23217017556640207</v>
+        <f>G14/F14-1</f>
+        <v>0.33949776133930309</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" si="17"/>
-        <v>-0.10860825351779591</v>
+        <f>H14/G14-1</f>
+        <v>-0.64699898270600209</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.11998408171386887</v>
+        <f>I14/H14-1</f>
+        <v>7.6986414162206751E-2</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" si="17"/>
-        <v>4.536302262229075E-2</v>
+        <f>J14/I14-1</f>
+        <v>1.3283639143730888</v>
       </c>
       <c r="K20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.19431225923408113</v>
+        <f>K14/J14-1</f>
+        <v>0.20653423083237565</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="17"/>
-        <v>-0.15866616070581541</v>
+        <f>L14/K14-1</f>
+        <v>-0.33297047217308473</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" si="17"/>
-        <v>5.3560354062130111E-2</v>
+        <f>M14/L14-1</f>
+        <v>5.6303549571603329E-2</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.14892706159362112</v>
+        <f>N14/M14-1</f>
+        <v>0.51525685592893011</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.30745225896599915</v>
+        <f>O14/N14-1</f>
+        <v>0.42187101707876629</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="17"/>
-        <v>-6.7685511738092674E-2</v>
+        <f>P14/O14-1</f>
+        <v>-0.1487092147723198</v>
       </c>
       <c r="Q20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.11103893622712158</v>
+        <f>Q14/P14-1</f>
+        <v>9.4450879225018491E-2</v>
       </c>
       <c r="R20" s="10">
-        <f t="shared" si="17"/>
-        <v>-2.3042267083949186E-3</v>
+        <f>R14/Q14-1</f>
+        <v>-0.11545122185876466</v>
       </c>
       <c r="S20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.16066873491899347</v>
+        <f>S14/R14-1</f>
+        <v>0.11866434631281275</v>
       </c>
       <c r="T20" s="10">
-        <f t="shared" si="17"/>
-        <v>-0.1711561878174096</v>
+        <f>T14/S14-1</f>
+        <v>-0.27418570734078751</v>
       </c>
       <c r="U20" s="10">
-        <f t="shared" si="17"/>
-        <v>3.2750465816253405E-2</v>
+        <f>U14/T14-1</f>
+        <v>-0.10421969189551239</v>
       </c>
       <c r="V20" s="10">
-        <f t="shared" si="17"/>
-        <v>-3.8442856151550853E-2</v>
+        <f>V14/U14-1</f>
+        <v>-0.34275459847465228</v>
       </c>
       <c r="W20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.1606047485025619</v>
+        <f>W14/V14-1</f>
+        <v>0.11513083048919226</v>
       </c>
       <c r="X20" s="10">
-        <f t="shared" si="17"/>
-        <v>-0.10943572205813767</v>
+        <f>X14/W14-1</f>
+        <v>0.16486431340542751</v>
       </c>
       <c r="Y20" s="10">
-        <f t="shared" si="17"/>
-        <v>0.1170884971199162</v>
+        <f>Y14/X14-1</f>
+        <v>0.36416184971098264</v>
       </c>
       <c r="Z20" s="10">
-        <f t="shared" si="17"/>
-        <v>6.7095846745210741E-2</v>
-      </c>
-      <c r="AA20" s="10"/>
+        <f>Z14/Y14-1</f>
+        <v>0.48728813559322037</v>
+      </c>
+      <c r="AA20" s="10">
+        <f>AA14/Z14-1</f>
+        <v>0.18682552015885356</v>
+      </c>
       <c r="AB20" s="10"/>
       <c r="AC20" s="10"/>
       <c r="AD20" s="10"/>
       <c r="AE20" s="10"/>
-      <c r="AF20" s="10"/>
+      <c r="AF20" s="1"/>
       <c r="AG20" s="10"/>
-      <c r="AH20" s="10"/>
-      <c r="AI20" s="10"/>
-      <c r="AJ20" s="1"/>
-      <c r="AK20" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL20" s="10"/>
+      <c r="AH20" s="10">
+        <f>AH14/AG14-1</f>
+        <v>-8.5742045178528015E-2</v>
+      </c>
+      <c r="AI20" s="10">
+        <f t="shared" ref="AI20:AR20" si="16">AI14/AH14-1</f>
+        <v>0.4394261424017003</v>
+      </c>
+      <c r="AJ20" s="10">
+        <f t="shared" si="16"/>
+        <v>0.69176818014027308</v>
+      </c>
+      <c r="AK20" s="10">
+        <f t="shared" si="16"/>
+        <v>0.41839406502291077</v>
+      </c>
+      <c r="AL20" s="10">
+        <f t="shared" si="16"/>
+        <v>0.24459656949465436</v>
+      </c>
       <c r="AM20" s="10">
-        <f t="shared" ref="AM20" si="18">AM5/AL5-1</f>
-        <v>0.5468657889565729</v>
+        <f t="shared" si="16"/>
+        <v>0.36654100488226926</v>
       </c>
       <c r="AN20" s="10">
-        <f t="shared" ref="AN20" si="19">AN5/AM5-1</f>
-        <v>0.58358739837398366</v>
+        <f t="shared" si="16"/>
+        <v>-0.16402858176555712</v>
       </c>
       <c r="AO20" s="10">
-        <f t="shared" ref="AO20" si="20">AO5/AN5-1</f>
-        <v>0.43815177282207607</v>
+        <f t="shared" si="16"/>
+        <v>0.57327562888828787</v>
       </c>
       <c r="AP20" s="10">
-        <f t="shared" ref="AP20" si="21">AP5/AO5-1</f>
-        <v>0.54161088799643009</v>
+        <f t="shared" si="16"/>
+        <v>0.35375833849116289</v>
       </c>
       <c r="AQ20" s="10">
-        <f t="shared" ref="AQ20" si="22">AQ5/AP5-1</f>
-        <v>0.47090961719371882</v>
+        <f t="shared" si="16"/>
+        <v>-0.40441960883921768</v>
       </c>
       <c r="AR20" s="10">
-        <f t="shared" ref="AR20" si="23">AR5/AQ5-1</f>
-        <v>0.37352716896661997</v>
-      </c>
-      <c r="AS20" s="10">
-        <f t="shared" ref="AS20:AV20" si="24">AS5/AR5-1</f>
-        <v>0.26610910132884413</v>
-      </c>
-      <c r="AT20" s="10">
-        <f t="shared" si="24"/>
-        <v>0.21596390228722573</v>
-      </c>
-      <c r="AU20" s="10">
-        <f t="shared" si="24"/>
-        <v>0.37182574303495608</v>
-      </c>
-      <c r="AV20" s="10">
-        <f t="shared" si="24"/>
-        <v>-1.1193175554782941E-2</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>0.65587683384510398</v>
+      </c>
+      <c r="AS20" s="10"/>
+      <c r="AT20" s="10"/>
+      <c r="AU20" s="10"/>
+      <c r="AV20" s="10"/>
       <c r="AW20" s="10"/>
       <c r="AX20" s="10"/>
       <c r="AY20" s="10"/>
@@ -4561,351 +4079,151 @@
       <c r="BS20" s="10"/>
       <c r="BT20" s="10"/>
       <c r="BU20" s="10"/>
-      <c r="BV20" s="10"/>
-      <c r="BW20" s="10"/>
-      <c r="BX20" s="10"/>
-      <c r="BY20" s="10"/>
-      <c r="BZ20" s="10"/>
     </row>
-    <row r="21" spans="3:79" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="10"/>
+    <row r="21" spans="3:74" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="E21" s="10">
-        <f>E14/D14-1</f>
-        <v>2.3656776263031309E-2</v>
-      </c>
-      <c r="F21" s="10">
-        <f t="shared" ref="F21:Z21" si="25">F14/E14-1</f>
-        <v>6.0712886799842991E-3</v>
-      </c>
-      <c r="G21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.33949776133930309</v>
-      </c>
-      <c r="H21" s="10">
-        <f t="shared" si="25"/>
-        <v>-0.64699898270600209</v>
-      </c>
-      <c r="I21" s="10">
-        <f t="shared" si="25"/>
-        <v>7.6986414162206751E-2</v>
-      </c>
-      <c r="J21" s="10">
-        <f t="shared" si="25"/>
-        <v>1.3283639143730888</v>
-      </c>
-      <c r="K21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.20653423083237565</v>
-      </c>
-      <c r="L21" s="10">
-        <f t="shared" si="25"/>
-        <v>-0.33297047217308473</v>
-      </c>
-      <c r="M21" s="10">
-        <f t="shared" si="25"/>
-        <v>5.6303549571603329E-2</v>
-      </c>
-      <c r="N21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.51525685592893011</v>
-      </c>
-      <c r="O21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.42187101707876629</v>
-      </c>
-      <c r="P21" s="10">
-        <f t="shared" si="25"/>
-        <v>-0.1487092147723198</v>
-      </c>
-      <c r="Q21" s="10">
-        <f t="shared" si="25"/>
-        <v>9.4450879225018491E-2</v>
-      </c>
-      <c r="R21" s="10">
-        <f t="shared" si="25"/>
-        <v>-0.11545122185876466</v>
-      </c>
-      <c r="S21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.11866434631281275</v>
-      </c>
-      <c r="T21" s="10">
-        <f t="shared" si="25"/>
-        <v>-0.27418570734078751</v>
-      </c>
-      <c r="U21" s="10">
-        <f t="shared" si="25"/>
-        <v>-0.10421969189551239</v>
-      </c>
-      <c r="V21" s="10">
-        <f t="shared" si="25"/>
-        <v>-0.34275459847465228</v>
-      </c>
-      <c r="W21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.11513083048919226</v>
-      </c>
-      <c r="X21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.16486431340542751</v>
-      </c>
-      <c r="Y21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.36416184971098264</v>
-      </c>
-      <c r="Z21" s="10">
-        <f t="shared" si="25"/>
-        <v>0.48728813559322037</v>
-      </c>
-      <c r="AA21" s="10"/>
-      <c r="AB21" s="10"/>
-      <c r="AC21" s="10"/>
-      <c r="AD21" s="10"/>
-      <c r="AE21" s="10"/>
-      <c r="AF21" s="10"/>
-      <c r="AG21" s="10"/>
-      <c r="AH21" s="10"/>
-      <c r="AI21" s="10"/>
-      <c r="AJ21" s="1"/>
-      <c r="AK21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL21" s="10"/>
-      <c r="AM21" s="10">
-        <f t="shared" ref="AM21" si="26">AM14/AL14-1</f>
-        <v>-8.5742045178528015E-2</v>
-      </c>
-      <c r="AN21" s="10">
-        <f t="shared" ref="AN21" si="27">AN14/AM14-1</f>
-        <v>0.4394261424017003</v>
-      </c>
-      <c r="AO21" s="10">
-        <f t="shared" ref="AO21" si="28">AO14/AN14-1</f>
-        <v>0.69176818014027308</v>
-      </c>
-      <c r="AP21" s="10">
-        <f t="shared" ref="AP21" si="29">AP14/AO14-1</f>
-        <v>0.41839406502291077</v>
-      </c>
-      <c r="AQ21" s="10">
-        <f t="shared" ref="AQ21" si="30">AQ14/AP14-1</f>
-        <v>0.24459656949465436</v>
-      </c>
-      <c r="AR21" s="10">
-        <f t="shared" ref="AR21" si="31">AR14/AQ14-1</f>
-        <v>0.36654100488226926</v>
-      </c>
-      <c r="AS21" s="10">
-        <f t="shared" ref="AS21:AV21" si="32">AS14/AR14-1</f>
-        <v>-0.16402858176555712</v>
-      </c>
-      <c r="AT21" s="10">
-        <f t="shared" si="32"/>
-        <v>0.57327562888828787</v>
-      </c>
-      <c r="AU21" s="10">
-        <f t="shared" si="32"/>
-        <v>0.35375833849116289</v>
-      </c>
-      <c r="AV21" s="10">
-        <f>AV14/AU14-1</f>
-        <v>-0.40441960883921768</v>
-      </c>
-      <c r="AW21" s="10"/>
-      <c r="AX21" s="10"/>
-      <c r="AY21" s="10"/>
-      <c r="AZ21" s="10"/>
-      <c r="BA21" s="10"/>
-      <c r="BB21" s="10"/>
-      <c r="BC21" s="10"/>
-      <c r="BD21" s="10"/>
-      <c r="BE21" s="10"/>
-      <c r="BF21" s="10"/>
-      <c r="BG21" s="10"/>
-      <c r="BH21" s="10"/>
-      <c r="BI21" s="10"/>
-      <c r="BJ21" s="10"/>
-      <c r="BK21" s="10"/>
-      <c r="BL21" s="10"/>
-      <c r="BM21" s="10"/>
-      <c r="BN21" s="10"/>
-      <c r="BO21" s="10"/>
-      <c r="BP21" s="10"/>
-      <c r="BQ21" s="10"/>
-      <c r="BR21" s="10"/>
-      <c r="BS21" s="10"/>
-      <c r="BT21" s="10"/>
-      <c r="BU21" s="10"/>
-      <c r="BV21" s="10"/>
-      <c r="BW21" s="10"/>
-      <c r="BX21" s="10"/>
-      <c r="BY21" s="10"/>
-      <c r="BZ21" s="10"/>
-    </row>
-    <row r="22" spans="3:79" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="11">
         <f>E7/D7-1</f>
         <v>0.12734584450402142</v>
       </c>
-      <c r="F22" s="11">
-        <f t="shared" ref="F22:Z22" si="33">F7/E7-1</f>
+      <c r="F21" s="10">
+        <f>F7/E7-1</f>
         <v>5.311137534680932E-2</v>
       </c>
-      <c r="G22" s="11">
-        <f t="shared" si="33"/>
+      <c r="G21" s="10">
+        <f>G7/F7-1</f>
         <v>7.4520135491155548E-2</v>
       </c>
-      <c r="H22" s="11">
-        <f t="shared" si="33"/>
+      <c r="H21" s="10">
+        <f>H7/G7-1</f>
         <v>1.7513134851139256E-3</v>
       </c>
-      <c r="I22" s="11">
-        <f t="shared" si="33"/>
+      <c r="I21" s="10">
+        <f>I7/H7-1</f>
         <v>0.15909090909090917</v>
       </c>
-      <c r="J22" s="11">
-        <f t="shared" si="33"/>
+      <c r="J21" s="10">
+        <f>J7/I7-1</f>
         <v>7.0286576168929082E-2</v>
       </c>
-      <c r="K22" s="11">
-        <f t="shared" si="33"/>
+      <c r="K21" s="10">
+        <f>K7/J7-1</f>
         <v>9.2728297632469037E-2</v>
       </c>
-      <c r="L22" s="11">
-        <f t="shared" si="33"/>
+      <c r="L21" s="10">
+        <f>L7/K7-1</f>
         <v>3.5594531854526767E-2</v>
       </c>
-      <c r="M22" s="11">
-        <f t="shared" si="33"/>
+      <c r="M21" s="10">
+        <f>M7/L7-1</f>
         <v>0.11133250311332499</v>
       </c>
-      <c r="N22" s="11">
-        <f t="shared" si="33"/>
+      <c r="N21" s="10">
+        <f>N7/M7-1</f>
         <v>6.7458538771851151E-2</v>
       </c>
-      <c r="O22" s="11">
-        <f t="shared" si="33"/>
+      <c r="O21" s="10">
+        <f>O7/N7-1</f>
         <v>9.3218559731261807E-2</v>
       </c>
-      <c r="P22" s="11">
-        <f t="shared" si="33"/>
+      <c r="P21" s="10">
+        <f>P7/O7-1</f>
         <v>-1.9204916458613885E-3</v>
       </c>
-      <c r="Q22" s="12">
-        <f t="shared" si="33"/>
+      <c r="Q21" s="10">
+        <f>Q7/P7-1</f>
         <v>0.17298441408504917</v>
       </c>
-      <c r="R22" s="11">
-        <f t="shared" si="33"/>
+      <c r="R21" s="10">
+        <f>R7/Q7-1</f>
         <v>3.6089238845144367E-2</v>
       </c>
-      <c r="S22" s="11">
-        <f t="shared" si="33"/>
+      <c r="S21" s="10">
+        <f>S7/R7-1</f>
         <v>0.11557948068397716</v>
       </c>
-      <c r="T22" s="11">
-        <f t="shared" si="33"/>
+      <c r="T21" s="10">
+        <f>T7/S7-1</f>
         <v>9.3812091967073519E-2</v>
       </c>
-      <c r="U22" s="11">
-        <f t="shared" si="33"/>
+      <c r="U21" s="10">
+        <f>U7/T7-1</f>
         <v>0.12754638640197213</v>
       </c>
-      <c r="V22" s="11">
-        <f t="shared" si="33"/>
+      <c r="V21" s="10">
+        <f>V7/U7-1</f>
         <v>5.5235903337169212E-2</v>
       </c>
-      <c r="W22" s="11">
-        <f t="shared" si="33"/>
+      <c r="W21" s="10">
+        <f>W7/V7-1</f>
         <v>6.5539803707742594E-2</v>
       </c>
-      <c r="X22" s="11">
-        <f t="shared" si="33"/>
+      <c r="X21" s="10">
+        <f>X7/W7-1</f>
         <v>-3.9914031317162979E-2</v>
       </c>
-      <c r="Y22" s="11">
-        <f t="shared" si="33"/>
+      <c r="Y21" s="10">
+        <f>Y7/X7-1</f>
         <v>-3.9441424155207683E-3</v>
       </c>
-      <c r="Z22" s="11">
-        <f t="shared" si="33"/>
+      <c r="Z21" s="10">
+        <f>Z7/Y7-1</f>
         <v>-1.1023116438356184E-2</v>
       </c>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
-      <c r="AD22" s="11"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11"/>
-      <c r="AI22" s="11"/>
-      <c r="AJ22" s="1"/>
-      <c r="AK22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL22" s="11"/>
-      <c r="AM22" s="11">
-        <f t="shared" ref="AM22:AR22" si="34">AM7/AL7-1</f>
+      <c r="AA21" s="10">
+        <f>AA7/Z7-1</f>
+        <v>0.13808029434043934</v>
+      </c>
+      <c r="AF21" s="14"/>
+      <c r="AH21" s="10">
+        <f>AH7/AG7-1</f>
         <v>1.1436740528949274E-2</v>
       </c>
-      <c r="AN22" s="11">
-        <f t="shared" si="34"/>
+      <c r="AI21" s="10">
+        <f t="shared" ref="AI21:AR21" si="17">AI7/AH7-1</f>
         <v>0.88409893992932864</v>
       </c>
-      <c r="AO22" s="11">
-        <f t="shared" si="34"/>
+      <c r="AJ21" s="10">
+        <f t="shared" si="17"/>
         <v>0.80645161290322576</v>
       </c>
-      <c r="AP22" s="11">
-        <f>AP7/AO7-1</f>
+      <c r="AK21" s="10">
+        <f t="shared" si="17"/>
         <v>0.22902823920265791</v>
       </c>
-      <c r="AQ22" s="11">
-        <f t="shared" si="34"/>
+      <c r="AL21" s="10">
+        <f t="shared" si="17"/>
         <v>0.31001858422030759</v>
       </c>
-      <c r="AR22" s="11">
-        <f t="shared" si="34"/>
+      <c r="AM21" s="10">
+        <f t="shared" si="17"/>
         <v>0.3248645860201187</v>
       </c>
-      <c r="AS22" s="11">
-        <f>AS7/AR7-1</f>
+      <c r="AN21" s="10">
+        <f t="shared" si="17"/>
         <v>0.32385865861968277</v>
       </c>
-      <c r="AT22" s="11">
-        <f t="shared" ref="AT22:AV22" si="35">AT7/AS7-1</f>
+      <c r="AO21" s="10">
+        <f t="shared" si="17"/>
         <v>0.35639705882352946</v>
       </c>
-      <c r="AU22" s="11">
-        <f t="shared" si="35"/>
+      <c r="AP21" s="10">
+        <f t="shared" si="17"/>
         <v>0.33653168536889466</v>
       </c>
-      <c r="AV22" s="11">
-        <f t="shared" si="35"/>
+      <c r="AQ21" s="10">
+        <f t="shared" si="17"/>
         <v>0.43329953356317175</v>
       </c>
-      <c r="AW22" s="11"/>
-      <c r="AX22" s="11"/>
-      <c r="AY22" s="11"/>
-      <c r="AZ22" s="11"/>
-      <c r="BA22" s="11"/>
-      <c r="BB22" s="11"/>
-      <c r="BC22" s="11"/>
-      <c r="BD22" s="11"/>
-      <c r="BE22" s="11"/>
-      <c r="BF22" s="11"/>
-      <c r="BG22" s="11"/>
-      <c r="BH22" s="11"/>
+      <c r="AR21" s="10">
+        <f t="shared" si="17"/>
+        <v>8.8997679551757303E-2</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A7:AC7 AE7:AI7 A5:AI6 A8:AI22 A1:XFD4 A23:XFD1048576 AJ5:XFD22">
+  <conditionalFormatting sqref="A7:AC7 AE7 A1:AE6 A22:XFD1048576 A8:AE21 AF1:XFD21">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>